<commit_message>
updated data to include R1 2023.
</commit_message>
<xml_diff>
--- a/AFL_ML/Data/Adelaide_stats.xlsx
+++ b/AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:JP102"/>
+  <dimension ref="A1:JQ102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1284,8 +1284,11 @@
       <c r="JO1" s="1" t="n">
         <v>10731</v>
       </c>
-      <c r="JP1" t="n">
+      <c r="JP1" s="1" t="n">
         <v>10741</v>
+      </c>
+      <c r="JQ1" t="n">
+        <v>10757</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -2116,8 +2119,11 @@
       <c r="JO2" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="JP2" t="n">
+      <c r="JP2" s="1" t="n">
         <v>2022</v>
+      </c>
+      <c r="JQ2" t="n">
+        <v>2023</v>
       </c>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="2">
@@ -2948,8 +2954,11 @@
       <c r="JO3" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="JP3" t="n">
+      <c r="JP3" s="1" t="n">
         <v>23</v>
+      </c>
+      <c r="JQ3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3780,7 +3789,10 @@
       <c r="JO4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JP4" t="n">
+      <c r="JP4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JQ4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4612,7 +4624,10 @@
       <c r="JO5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JP5" t="n">
+      <c r="JP5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JQ5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5444,8 +5459,11 @@
       <c r="JO6" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="JP6" t="n">
+      <c r="JP6" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="JQ6" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -6276,8 +6294,11 @@
       <c r="JO7" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="JP7" t="n">
+      <c r="JP7" s="1" t="n">
         <v>111</v>
+      </c>
+      <c r="JQ7" t="n">
+        <v>106</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -7108,8 +7129,11 @@
       <c r="JO8" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="JP8" t="n">
+      <c r="JP8" s="1" t="n">
         <v>-56</v>
+      </c>
+      <c r="JQ8" t="n">
+        <v>-16</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -7940,7 +7964,10 @@
       <c r="JO9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JP9" t="n">
+      <c r="JP9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JQ9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8772,8 +8799,11 @@
       <c r="JO10" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="JP10" t="n">
+      <c r="JP10" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="JQ10" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -9604,8 +9634,11 @@
       <c r="JO11" s="1" t="n">
         <v>212</v>
       </c>
-      <c r="JP11" t="n">
+      <c r="JP11" s="1" t="n">
         <v>166</v>
+      </c>
+      <c r="JQ11" t="n">
+        <v>217</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -10436,8 +10469,11 @@
       <c r="JO12" s="1" t="n">
         <v>137</v>
       </c>
-      <c r="JP12" t="n">
+      <c r="JP12" s="1" t="n">
         <v>121</v>
+      </c>
+      <c r="JQ12" t="n">
+        <v>101</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -11268,8 +11304,11 @@
       <c r="JO13" s="1" t="n">
         <v>349</v>
       </c>
-      <c r="JP13" t="n">
+      <c r="JP13" s="1" t="n">
         <v>287</v>
+      </c>
+      <c r="JQ13" t="n">
+        <v>318</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -12100,8 +12139,11 @@
       <c r="JO14" s="1" t="n">
         <v>1.55</v>
       </c>
-      <c r="JP14" t="n">
+      <c r="JP14" s="1" t="n">
         <v>1.37</v>
+      </c>
+      <c r="JQ14" t="n">
+        <v>2.15</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -12932,8 +12974,11 @@
       <c r="JO15" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="JP15" t="n">
+      <c r="JP15" s="1" t="n">
         <v>48</v>
+      </c>
+      <c r="JQ15" t="n">
+        <v>102</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -13764,8 +13809,11 @@
       <c r="JO16" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="JP16" t="n">
+      <c r="JP16" s="1" t="n">
         <v>70</v>
+      </c>
+      <c r="JQ16" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -14596,8 +14644,11 @@
       <c r="JO17" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="JP17" t="n">
+      <c r="JP17" s="1" t="n">
         <v>59</v>
+      </c>
+      <c r="JQ17" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -15428,8 +15479,11 @@
       <c r="JO18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="JP18" t="n">
+      <c r="JP18" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="JQ18" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -16260,8 +16314,11 @@
       <c r="JO19" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="JP19" t="n">
+      <c r="JP19" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="JQ19" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -17092,8 +17149,11 @@
       <c r="JO20" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="JP20" t="n">
+      <c r="JP20" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="JQ20" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -17924,8 +17984,11 @@
       <c r="JO21" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="JP21" t="n">
+      <c r="JP21" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="JQ21" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -18756,8 +18819,11 @@
       <c r="JO22" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="JP22" t="n">
+      <c r="JP22" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="JQ22" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -19588,8 +19654,11 @@
       <c r="JO23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="JP23" t="n">
+      <c r="JP23" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="JQ23" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -20420,8 +20489,11 @@
       <c r="JO24" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="JP24" t="n">
+      <c r="JP24" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="JQ24" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -21252,8 +21324,11 @@
       <c r="JO25" s="1" t="n">
         <v>53.6</v>
       </c>
-      <c r="JP25" t="n">
+      <c r="JP25" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="JQ25" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -22084,8 +22159,11 @@
       <c r="JO26" s="1" t="n">
         <v>23.27</v>
       </c>
-      <c r="JP26" t="n">
+      <c r="JP26" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="JQ26" t="n">
+        <v>26.5</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -22916,8 +22994,11 @@
       <c r="JO27" s="1" t="n">
         <v>12.46</v>
       </c>
-      <c r="JP27" t="n">
+      <c r="JP27" s="1" t="n">
         <v>14.35</v>
+      </c>
+      <c r="JQ27" t="n">
+        <v>10.6</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -23748,8 +23829,11 @@
       <c r="JO28" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="JP28" t="n">
+      <c r="JP28" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="JQ28" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -24580,8 +24664,11 @@
       <c r="JO29" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="JP29" t="n">
+      <c r="JP29" s="1" t="n">
         <v>65</v>
+      </c>
+      <c r="JQ29" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -25412,8 +25499,11 @@
       <c r="JO30" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="JP30" t="n">
+      <c r="JP30" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="JQ30" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -26244,8 +26334,11 @@
       <c r="JO31" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="JP31" t="n">
+      <c r="JP31" s="1" t="n">
         <v>48</v>
+      </c>
+      <c r="JQ31" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -27076,8 +27169,11 @@
       <c r="JO32" s="1" t="n">
         <v>1.86</v>
       </c>
-      <c r="JP32" t="n">
+      <c r="JP32" s="1" t="n">
         <v>2.4</v>
+      </c>
+      <c r="JQ32" t="n">
+        <v>1.73</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -27908,8 +28004,11 @@
       <c r="JO33" s="1" t="n">
         <v>3.47</v>
       </c>
-      <c r="JP33" t="n">
+      <c r="JP33" s="1" t="n">
         <v>6.86</v>
+      </c>
+      <c r="JQ33" t="n">
+        <v>4.33</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -28740,8 +28839,11 @@
       <c r="JO34" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="JP34" t="n">
+      <c r="JP34" s="1" t="n">
         <v>31.2</v>
+      </c>
+      <c r="JQ34" t="n">
+        <v>53.8</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -29572,8 +29674,11 @@
       <c r="JO35" s="1" t="n">
         <v>28.8</v>
       </c>
-      <c r="JP35" t="n">
+      <c r="JP35" s="1" t="n">
         <v>14.6</v>
+      </c>
+      <c r="JQ35" t="n">
+        <v>23.1</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -30404,8 +30509,11 @@
       <c r="JO36" s="1" t="n">
         <v>186.8</v>
       </c>
-      <c r="JP36" t="n">
+      <c r="JP36" s="1" t="n">
         <v>186.9</v>
+      </c>
+      <c r="JQ36" t="n">
+        <v>188.1</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -31236,8 +31344,11 @@
       <c r="JO37" s="1" t="n">
         <v>87.09999999999999</v>
       </c>
-      <c r="JP37" t="n">
+      <c r="JP37" s="1" t="n">
         <v>87.3</v>
+      </c>
+      <c r="JQ37" t="n">
+        <v>88</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -32068,8 +32179,11 @@
       <c r="JO38" s="1" t="n">
         <v>24.8</v>
       </c>
-      <c r="JP38" t="n">
+      <c r="JP38" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="JQ38" t="n">
+        <v>24.91</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -32900,8 +33014,11 @@
       <c r="JO39" s="1" t="n">
         <v>66.5</v>
       </c>
-      <c r="JP39" t="n">
+      <c r="JP39" s="1" t="n">
         <v>68.8</v>
+      </c>
+      <c r="JQ39" t="n">
+        <v>75.7</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -33732,8 +33849,11 @@
       <c r="JO40" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="JP40" t="n">
+      <c r="JP40" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="JQ40" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="2">
@@ -34564,8 +34684,11 @@
       <c r="JO41" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JP41" t="n">
+      <c r="JP41" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="JQ41" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="2">
@@ -35396,7 +35519,10 @@
       <c r="JO42" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JP42" t="n">
+      <c r="JP42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JQ42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -36228,8 +36354,11 @@
       <c r="JO43" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JP43" t="n">
+      <c r="JP43" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="JQ43" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="44" ht="13.8" customHeight="1" s="2">
@@ -37060,8 +37189,11 @@
       <c r="JO44" s="1" t="n">
         <v>127</v>
       </c>
-      <c r="JP44" t="n">
+      <c r="JP44" s="1" t="n">
         <v>146</v>
+      </c>
+      <c r="JQ44" t="n">
+        <v>111</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -37892,8 +38024,11 @@
       <c r="JO45" s="1" t="n">
         <v>213</v>
       </c>
-      <c r="JP45" t="n">
+      <c r="JP45" s="1" t="n">
         <v>129</v>
+      </c>
+      <c r="JQ45" t="n">
+        <v>199</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -38724,8 +38859,11 @@
       <c r="JO46" s="1" t="n">
         <v>272</v>
       </c>
-      <c r="JP46" t="n">
+      <c r="JP46" s="1" t="n">
         <v>181</v>
+      </c>
+      <c r="JQ46" t="n">
+        <v>242</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -39556,8 +39694,11 @@
       <c r="JO47" s="1" t="n">
         <v>77.90000000000001</v>
       </c>
-      <c r="JP47" t="n">
+      <c r="JP47" s="1" t="n">
         <v>63.1</v>
+      </c>
+      <c r="JQ47" t="n">
+        <v>76.09999999999999</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -40388,8 +40529,11 @@
       <c r="JO48" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="JP48" t="n">
+      <c r="JP48" s="1" t="n">
         <v>65</v>
+      </c>
+      <c r="JQ48" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -41220,8 +41364,11 @@
       <c r="JO49" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="JP49" t="n">
+      <c r="JP49" s="1" t="n">
         <v>19</v>
+      </c>
+      <c r="JQ49" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -42052,8 +42199,11 @@
       <c r="JO50" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="JP50" t="n">
+      <c r="JP50" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="JQ50" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -42884,8 +43034,11 @@
       <c r="JO51" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="JP51" t="n">
+      <c r="JP51" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="JQ51" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -43716,8 +43869,11 @@
       <c r="JO52" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="JP52" t="n">
+      <c r="JP52" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="JQ52" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -44548,8 +44704,11 @@
       <c r="JO53" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="JP53" t="n">
+      <c r="JP53" s="1" t="n">
         <v>60</v>
+      </c>
+      <c r="JQ53" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -45380,8 +45539,11 @@
       <c r="JO54" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="JP54" t="n">
+      <c r="JP54" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="JQ54" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -46212,8 +46374,11 @@
       <c r="JO55" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="JP55" t="n">
+      <c r="JP55" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="JQ55" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -47044,8 +47209,11 @@
       <c r="JO56" s="1" t="n">
         <v>86.7</v>
       </c>
-      <c r="JP56" t="n">
+      <c r="JP56" s="1" t="n">
         <v>71.40000000000001</v>
+      </c>
+      <c r="JQ56" t="n">
+        <v>83.3</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -47876,8 +48044,11 @@
       <c r="JO57" s="1" t="n">
         <v>203</v>
       </c>
-      <c r="JP57" t="n">
+      <c r="JP57" s="1" t="n">
         <v>237</v>
+      </c>
+      <c r="JQ57" t="n">
+        <v>208</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -48708,8 +48879,11 @@
       <c r="JO58" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="JP58" t="n">
+      <c r="JP58" s="1" t="n">
         <v>164</v>
+      </c>
+      <c r="JQ58" t="n">
+        <v>167</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -49540,8 +49714,11 @@
       <c r="JO59" s="1" t="n">
         <v>353</v>
       </c>
-      <c r="JP59" t="n">
+      <c r="JP59" s="1" t="n">
         <v>401</v>
+      </c>
+      <c r="JQ59" t="n">
+        <v>375</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -50372,8 +50549,11 @@
       <c r="JO60" s="1" t="n">
         <v>1.35</v>
       </c>
-      <c r="JP60" t="n">
+      <c r="JP60" s="1" t="n">
         <v>1.45</v>
+      </c>
+      <c r="JQ60" t="n">
+        <v>1.25</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -51204,8 +51384,11 @@
       <c r="JO61" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="JP61" t="n">
+      <c r="JP61" s="1" t="n">
         <v>97</v>
+      </c>
+      <c r="JQ61" t="n">
+        <v>88</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -52036,8 +52219,11 @@
       <c r="JO62" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="JP62" t="n">
+      <c r="JP62" s="1" t="n">
         <v>68</v>
+      </c>
+      <c r="JQ62" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -52868,8 +53054,11 @@
       <c r="JO63" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="JP63" t="n">
+      <c r="JP63" s="1" t="n">
         <v>23</v>
+      </c>
+      <c r="JQ63" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -53700,8 +53889,11 @@
       <c r="JO64" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="JP64" t="n">
+      <c r="JP64" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="JQ64" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -54532,8 +54724,11 @@
       <c r="JO65" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="JP65" t="n">
+      <c r="JP65" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="JQ65" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -55364,8 +55559,11 @@
       <c r="JO66" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="JP66" t="n">
+      <c r="JP66" s="1" t="n">
         <v>16</v>
+      </c>
+      <c r="JQ66" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -56196,8 +56394,11 @@
       <c r="JO67" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JP67" t="n">
+      <c r="JP67" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="JQ67" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -57028,8 +57229,11 @@
       <c r="JO68" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="JP68" t="n">
+      <c r="JP68" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="JQ68" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -57860,8 +58064,11 @@
       <c r="JO69" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JP69" t="n">
+      <c r="JP69" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="JQ69" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -58692,7 +58899,10 @@
       <c r="JO70" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="JP70" t="n">
+      <c r="JP70" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="JQ70" t="n">
         <v>31</v>
       </c>
     </row>
@@ -59524,8 +59734,11 @@
       <c r="JO71" s="1" t="n">
         <v>41.7</v>
       </c>
-      <c r="JP71" t="n">
+      <c r="JP71" s="1" t="n">
         <v>51.6</v>
+      </c>
+      <c r="JQ71" t="n">
+        <v>48.4</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -60356,8 +60569,11 @@
       <c r="JO72" s="1" t="n">
         <v>35.3</v>
       </c>
-      <c r="JP72" t="n">
+      <c r="JP72" s="1" t="n">
         <v>25.06</v>
+      </c>
+      <c r="JQ72" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -61188,8 +61404,11 @@
       <c r="JO73" s="1" t="n">
         <v>14.71</v>
       </c>
-      <c r="JP73" t="n">
+      <c r="JP73" s="1" t="n">
         <v>12.94</v>
+      </c>
+      <c r="JQ73" t="n">
+        <v>12.1</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -62020,8 +62239,11 @@
       <c r="JO74" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="JP74" t="n">
+      <c r="JP74" s="1" t="n">
         <v>45</v>
+      </c>
+      <c r="JQ74" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -62852,8 +63074,11 @@
       <c r="JO75" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="JP75" t="n">
+      <c r="JP75" s="1" t="n">
         <v>54</v>
+      </c>
+      <c r="JQ75" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -63684,8 +63909,11 @@
       <c r="JO76" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="JP76" t="n">
+      <c r="JP76" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="JQ76" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -64516,8 +64744,11 @@
       <c r="JO77" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="JP77" t="n">
+      <c r="JP77" s="1" t="n">
         <v>61</v>
+      </c>
+      <c r="JQ77" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -65348,8 +65579,11 @@
       <c r="JO78" s="1" t="n">
         <v>2.46</v>
       </c>
-      <c r="JP78" t="n">
+      <c r="JP78" s="1" t="n">
         <v>1.97</v>
+      </c>
+      <c r="JQ78" t="n">
+        <v>1.94</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -66180,8 +66414,11 @@
       <c r="JO79" s="1" t="n">
         <v>5.9</v>
       </c>
-      <c r="JP79" t="n">
+      <c r="JP79" s="1" t="n">
         <v>3.81</v>
+      </c>
+      <c r="JQ79" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -67012,8 +67249,11 @@
       <c r="JO80" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="JP80" t="n">
+      <c r="JP80" s="1" t="n">
         <v>42.6</v>
+      </c>
+      <c r="JQ80" t="n">
+        <v>46.7</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -67844,8 +68084,11 @@
       <c r="JO81" s="1" t="n">
         <v>16.9</v>
       </c>
-      <c r="JP81" t="n">
+      <c r="JP81" s="1" t="n">
         <v>26.2</v>
+      </c>
+      <c r="JQ81" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -68676,8 +68919,11 @@
       <c r="JO82" s="1" t="n">
         <v>189</v>
       </c>
-      <c r="JP82" t="n">
+      <c r="JP82" s="1" t="n">
         <v>187.4</v>
+      </c>
+      <c r="JQ82" t="n">
+        <v>188.6</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -69508,8 +69754,11 @@
       <c r="JO83" s="1" t="n">
         <v>85.2</v>
       </c>
-      <c r="JP83" t="n">
+      <c r="JP83" s="1" t="n">
         <v>85.40000000000001</v>
+      </c>
+      <c r="JQ83" t="n">
+        <v>87</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -70340,8 +70589,11 @@
       <c r="JO84" s="1" t="n">
         <v>25.24</v>
       </c>
-      <c r="JP84" t="n">
+      <c r="JP84" s="1" t="n">
         <v>25.58</v>
+      </c>
+      <c r="JQ84" t="n">
+        <v>26.8</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -71172,8 +71424,11 @@
       <c r="JO85" s="1" t="n">
         <v>92.7</v>
       </c>
-      <c r="JP85" t="n">
+      <c r="JP85" s="1" t="n">
         <v>112.1</v>
+      </c>
+      <c r="JQ85" t="n">
+        <v>95.5</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -72004,8 +72259,11 @@
       <c r="JO86" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JP86" t="n">
+      <c r="JP86" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="JQ86" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -72836,8 +73094,11 @@
       <c r="JO87" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JP87" t="n">
+      <c r="JP87" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="JQ87" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -73668,8 +73929,11 @@
       <c r="JO88" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JP88" t="n">
+      <c r="JP88" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="JQ88" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -74500,7 +74764,10 @@
       <c r="JO89" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="JP89" t="n">
+      <c r="JP89" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JQ89" t="n">
         <v>6</v>
       </c>
     </row>
@@ -75332,8 +75599,11 @@
       <c r="JO90" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="JP90" t="n">
+      <c r="JP90" s="1" t="n">
         <v>146</v>
+      </c>
+      <c r="JQ90" t="n">
+        <v>129</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -76164,7 +76434,10 @@
       <c r="JO91" s="1" t="n">
         <v>221</v>
       </c>
-      <c r="JP91" t="n">
+      <c r="JP91" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="JQ91" t="n">
         <v>236</v>
       </c>
     </row>
@@ -76996,7 +77269,10 @@
       <c r="JO92" s="1" t="n">
         <v>267</v>
       </c>
-      <c r="JP92" t="n">
+      <c r="JP92" s="1" t="n">
+        <v>287</v>
+      </c>
+      <c r="JQ92" t="n">
         <v>287</v>
       </c>
     </row>
@@ -77828,8 +78104,11 @@
       <c r="JO93" s="1" t="n">
         <v>75.59999999999999</v>
       </c>
-      <c r="JP93" t="n">
+      <c r="JP93" s="1" t="n">
         <v>71.59999999999999</v>
+      </c>
+      <c r="JQ93" t="n">
+        <v>76.5</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -78660,8 +78939,11 @@
       <c r="JO94" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="JP94" t="n">
+      <c r="JP94" s="1" t="n">
         <v>54</v>
+      </c>
+      <c r="JQ94" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -79492,8 +79774,11 @@
       <c r="JO95" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="JP95" t="n">
+      <c r="JP95" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="JQ95" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -80324,8 +80609,11 @@
       <c r="JO96" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JP96" t="n">
+      <c r="JP96" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="JQ96" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -81156,8 +81444,11 @@
       <c r="JO97" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="JP97" t="n">
+      <c r="JP97" s="1" t="n">
         <v>45</v>
+      </c>
+      <c r="JQ97" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -81988,8 +82279,11 @@
       <c r="JO98" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="JP98" t="n">
+      <c r="JP98" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="JQ98" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -82820,8 +83114,11 @@
       <c r="JO99" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="JP99" t="n">
+      <c r="JP99" s="1" t="n">
         <v>54</v>
+      </c>
+      <c r="JQ99" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -83652,8 +83949,11 @@
       <c r="JO100" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JP100" t="n">
+      <c r="JP100" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="JQ100" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -84484,8 +84784,11 @@
       <c r="JO101" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JP101" t="n">
+      <c r="JP101" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="JQ101" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -85316,8 +85619,11 @@
       <c r="JO102" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="JP102" t="n">
+      <c r="JP102" s="1" t="n">
         <v>68.8</v>
+      </c>
+      <c r="JQ102" t="n">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
round 3 data added to files. recorded tips
</commit_message>
<xml_diff>
--- a/AFL_ML/Data/Adelaide_stats.xlsx
+++ b/AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:JR102"/>
+  <dimension ref="A1:JS102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1290,8 +1290,11 @@
       <c r="JQ1" s="1" t="n">
         <v>10757</v>
       </c>
-      <c r="JR1" t="n">
+      <c r="JR1" s="1" t="n">
         <v>10763</v>
+      </c>
+      <c r="JS1" t="n">
+        <v>10774</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -2128,7 +2131,10 @@
       <c r="JQ2" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="JR2" t="n">
+      <c r="JR2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="JS2" t="n">
         <v>2023</v>
       </c>
     </row>
@@ -2966,8 +2972,11 @@
       <c r="JQ3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JR3" t="n">
+      <c r="JR3" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="JS3" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3804,8 +3813,11 @@
       <c r="JQ4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JR4" t="n">
+      <c r="JR4" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="JS4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -4642,7 +4654,10 @@
       <c r="JQ5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JR5" t="n">
+      <c r="JR5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JS5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5480,8 +5495,11 @@
       <c r="JQ6" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="JR6" t="n">
+      <c r="JR6" s="1" t="n">
         <v>76</v>
+      </c>
+      <c r="JS6" t="n">
+        <v>117</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -6318,8 +6336,11 @@
       <c r="JQ7" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="JR7" t="n">
+      <c r="JR7" s="1" t="n">
         <v>108</v>
+      </c>
+      <c r="JS7" t="n">
+        <v>86</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -7156,8 +7177,11 @@
       <c r="JQ8" s="1" t="n">
         <v>-16</v>
       </c>
-      <c r="JR8" t="n">
+      <c r="JR8" s="1" t="n">
         <v>-32</v>
+      </c>
+      <c r="JS8" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -7994,8 +8018,11 @@
       <c r="JQ9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JR9" t="n">
+      <c r="JR9" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="JS9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="2">
@@ -8832,8 +8859,11 @@
       <c r="JQ10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JR10" t="n">
+      <c r="JR10" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="JS10" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -9670,8 +9700,11 @@
       <c r="JQ11" s="1" t="n">
         <v>217</v>
       </c>
-      <c r="JR11" t="n">
+      <c r="JR11" s="1" t="n">
         <v>216</v>
+      </c>
+      <c r="JS11" t="n">
+        <v>212</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -10508,8 +10541,11 @@
       <c r="JQ12" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="JR12" t="n">
+      <c r="JR12" s="1" t="n">
         <v>142</v>
+      </c>
+      <c r="JS12" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -11346,8 +11382,11 @@
       <c r="JQ13" s="1" t="n">
         <v>318</v>
       </c>
-      <c r="JR13" t="n">
+      <c r="JR13" s="1" t="n">
         <v>358</v>
+      </c>
+      <c r="JS13" t="n">
+        <v>332</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -12184,8 +12223,11 @@
       <c r="JQ14" s="1" t="n">
         <v>2.15</v>
       </c>
-      <c r="JR14" t="n">
+      <c r="JR14" s="1" t="n">
         <v>1.52</v>
+      </c>
+      <c r="JS14" t="n">
+        <v>1.77</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -13022,8 +13064,11 @@
       <c r="JQ15" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="JR15" t="n">
+      <c r="JR15" s="1" t="n">
         <v>94</v>
+      </c>
+      <c r="JS15" t="n">
+        <v>88</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -13860,8 +13905,11 @@
       <c r="JQ16" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="JR16" t="n">
+      <c r="JR16" s="1" t="n">
         <v>60</v>
+      </c>
+      <c r="JS16" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -14698,8 +14746,11 @@
       <c r="JQ17" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="JR17" t="n">
+      <c r="JR17" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="JS17" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -15536,8 +15587,11 @@
       <c r="JQ18" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="JR18" t="n">
+      <c r="JR18" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="JS18" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -16374,8 +16428,11 @@
       <c r="JQ19" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="JR19" t="n">
+      <c r="JR19" s="1" t="n">
         <v>16</v>
+      </c>
+      <c r="JS19" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -17212,8 +17269,11 @@
       <c r="JQ20" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="JR20" t="n">
+      <c r="JR20" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="JS20" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -18050,8 +18110,11 @@
       <c r="JQ21" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="JR21" t="n">
+      <c r="JR21" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="JS21" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -18888,8 +18951,11 @@
       <c r="JQ22" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="JR22" t="n">
+      <c r="JR22" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="JS22" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -19726,8 +19792,11 @@
       <c r="JQ23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="JR23" t="n">
+      <c r="JR23" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="JS23" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -20564,8 +20633,11 @@
       <c r="JQ24" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="JR24" t="n">
+      <c r="JR24" s="1" t="n">
         <v>26</v>
+      </c>
+      <c r="JS24" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -21402,8 +21474,11 @@
       <c r="JQ25" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="JR25" t="n">
+      <c r="JR25" s="1" t="n">
         <v>38.5</v>
+      </c>
+      <c r="JS25" t="n">
+        <v>66.7</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -22240,8 +22315,11 @@
       <c r="JQ26" s="1" t="n">
         <v>26.5</v>
       </c>
-      <c r="JR26" t="n">
+      <c r="JR26" s="1" t="n">
         <v>35.8</v>
+      </c>
+      <c r="JS26" t="n">
+        <v>18.44</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -23078,8 +23156,11 @@
       <c r="JQ27" s="1" t="n">
         <v>10.6</v>
       </c>
-      <c r="JR27" t="n">
+      <c r="JR27" s="1" t="n">
         <v>13.77</v>
+      </c>
+      <c r="JS27" t="n">
+        <v>12.3</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -23916,8 +23997,11 @@
       <c r="JQ28" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="JR28" t="n">
+      <c r="JR28" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="JS28" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -24754,8 +24838,11 @@
       <c r="JQ29" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="JR29" t="n">
+      <c r="JR29" s="1" t="n">
         <v>54</v>
+      </c>
+      <c r="JS29" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -25592,8 +25679,11 @@
       <c r="JQ30" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="JR30" t="n">
+      <c r="JR30" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="JS30" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -26430,8 +26520,11 @@
       <c r="JQ31" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="JR31" t="n">
+      <c r="JR31" s="1" t="n">
         <v>53</v>
+      </c>
+      <c r="JS31" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -27268,8 +27361,11 @@
       <c r="JQ32" s="1" t="n">
         <v>1.73</v>
       </c>
-      <c r="JR32" t="n">
+      <c r="JR32" s="1" t="n">
         <v>2.04</v>
+      </c>
+      <c r="JS32" t="n">
+        <v>2.19</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -28106,8 +28202,11 @@
       <c r="JQ33" s="1" t="n">
         <v>4.33</v>
       </c>
-      <c r="JR33" t="n">
+      <c r="JR33" s="1" t="n">
         <v>5.3</v>
+      </c>
+      <c r="JS33" t="n">
+        <v>3.28</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -28944,8 +29043,11 @@
       <c r="JQ34" s="1" t="n">
         <v>53.8</v>
       </c>
-      <c r="JR34" t="n">
+      <c r="JR34" s="1" t="n">
         <v>43.4</v>
+      </c>
+      <c r="JS34" t="n">
+        <v>44.1</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -29782,8 +29884,11 @@
       <c r="JQ35" s="1" t="n">
         <v>23.1</v>
       </c>
-      <c r="JR35" t="n">
+      <c r="JR35" s="1" t="n">
         <v>18.9</v>
+      </c>
+      <c r="JS35" t="n">
+        <v>30.5</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -30620,7 +30725,10 @@
       <c r="JQ36" s="1" t="n">
         <v>188.1</v>
       </c>
-      <c r="JR36" t="n">
+      <c r="JR36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="JS36" t="n">
         <v>187.3</v>
       </c>
     </row>
@@ -31458,8 +31566,11 @@
       <c r="JQ37" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="JR37" t="n">
+      <c r="JR37" s="1" t="n">
         <v>87.59999999999999</v>
+      </c>
+      <c r="JS37" t="n">
+        <v>87.5</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -32296,8 +32407,11 @@
       <c r="JQ38" s="1" t="n">
         <v>24.91</v>
       </c>
-      <c r="JR38" t="n">
+      <c r="JR38" s="1" t="n">
         <v>24.49</v>
+      </c>
+      <c r="JS38" t="n">
+        <v>24.58</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -33134,8 +33248,11 @@
       <c r="JQ39" s="1" t="n">
         <v>75.7</v>
       </c>
-      <c r="JR39" t="n">
+      <c r="JR39" s="1" t="n">
         <v>74.90000000000001</v>
+      </c>
+      <c r="JS39" t="n">
+        <v>77</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -33972,8 +34089,11 @@
       <c r="JQ40" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="JR40" t="n">
+      <c r="JR40" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="JS40" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="2">
@@ -34810,8 +34930,11 @@
       <c r="JQ41" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="JR41" t="n">
+      <c r="JR41" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="JS41" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="2">
@@ -35648,7 +35771,10 @@
       <c r="JQ42" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JR42" t="n">
+      <c r="JR42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JS42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -36486,7 +36612,10 @@
       <c r="JQ43" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JR43" t="n">
+      <c r="JR43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JS43" t="n">
         <v>4</v>
       </c>
     </row>
@@ -37324,8 +37453,11 @@
       <c r="JQ44" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="JR44" t="n">
+      <c r="JR44" s="1" t="n">
         <v>139</v>
+      </c>
+      <c r="JS44" t="n">
+        <v>146</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -38162,8 +38294,11 @@
       <c r="JQ45" s="1" t="n">
         <v>199</v>
       </c>
-      <c r="JR45" t="n">
+      <c r="JR45" s="1" t="n">
         <v>213</v>
+      </c>
+      <c r="JS45" t="n">
+        <v>183</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -39000,8 +39135,11 @@
       <c r="JQ46" s="1" t="n">
         <v>242</v>
       </c>
-      <c r="JR46" t="n">
+      <c r="JR46" s="1" t="n">
         <v>253</v>
+      </c>
+      <c r="JS46" t="n">
+        <v>251</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -39838,8 +39976,11 @@
       <c r="JQ47" s="1" t="n">
         <v>76.09999999999999</v>
       </c>
-      <c r="JR47" t="n">
+      <c r="JR47" s="1" t="n">
         <v>70.7</v>
+      </c>
+      <c r="JS47" t="n">
+        <v>75.59999999999999</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -40676,8 +40817,11 @@
       <c r="JQ48" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="JR48" t="n">
+      <c r="JR48" s="1" t="n">
         <v>54</v>
+      </c>
+      <c r="JS48" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -41514,8 +41658,11 @@
       <c r="JQ49" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JR49" t="n">
+      <c r="JR49" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="JS49" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -42352,8 +42499,11 @@
       <c r="JQ50" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="JR50" t="n">
+      <c r="JR50" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="JS50" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -43190,8 +43340,11 @@
       <c r="JQ51" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="JR51" t="n">
+      <c r="JR51" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="JS51" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -44028,8 +44181,11 @@
       <c r="JQ52" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="JR52" t="n">
+      <c r="JR52" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="JS52" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -44866,8 +45022,11 @@
       <c r="JQ53" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="JR53" t="n">
+      <c r="JR53" s="1" t="n">
         <v>47</v>
+      </c>
+      <c r="JS53" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -45704,8 +45863,11 @@
       <c r="JQ54" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JR54" t="n">
+      <c r="JR54" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="JS54" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -46542,8 +46704,11 @@
       <c r="JQ55" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="JR55" t="n">
+      <c r="JR55" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="JS55" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -47380,8 +47545,11 @@
       <c r="JQ56" s="1" t="n">
         <v>83.3</v>
       </c>
-      <c r="JR56" t="n">
+      <c r="JR56" s="1" t="n">
         <v>90</v>
+      </c>
+      <c r="JS56" t="n">
+        <v>72.2</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -48218,8 +48386,11 @@
       <c r="JQ57" s="1" t="n">
         <v>208</v>
       </c>
-      <c r="JR57" t="n">
+      <c r="JR57" s="1" t="n">
         <v>209</v>
+      </c>
+      <c r="JS57" t="n">
+        <v>188</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -49056,8 +49227,11 @@
       <c r="JQ58" s="1" t="n">
         <v>167</v>
       </c>
-      <c r="JR58" t="n">
+      <c r="JR58" s="1" t="n">
         <v>139</v>
+      </c>
+      <c r="JS58" t="n">
+        <v>109</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -49894,8 +50068,11 @@
       <c r="JQ59" s="1" t="n">
         <v>375</v>
       </c>
-      <c r="JR59" t="n">
+      <c r="JR59" s="1" t="n">
         <v>348</v>
+      </c>
+      <c r="JS59" t="n">
+        <v>297</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -50732,8 +50909,11 @@
       <c r="JQ60" s="1" t="n">
         <v>1.25</v>
       </c>
-      <c r="JR60" t="n">
+      <c r="JR60" s="1" t="n">
         <v>1.5</v>
+      </c>
+      <c r="JS60" t="n">
+        <v>1.72</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -51570,8 +51750,11 @@
       <c r="JQ61" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="JR61" t="n">
+      <c r="JR61" s="1" t="n">
         <v>94</v>
+      </c>
+      <c r="JS61" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -52408,8 +52591,11 @@
       <c r="JQ62" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="JR62" t="n">
+      <c r="JR62" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="JS62" t="n">
+        <v>76</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -53246,8 +53432,11 @@
       <c r="JQ63" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="JR63" t="n">
+      <c r="JR63" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="JS63" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -54084,8 +54273,11 @@
       <c r="JQ64" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="JR64" t="n">
+      <c r="JR64" s="1" t="n">
         <v>16</v>
+      </c>
+      <c r="JS64" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -54922,8 +55114,11 @@
       <c r="JQ65" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="JR65" t="n">
+      <c r="JR65" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="JS65" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -55760,8 +55955,11 @@
       <c r="JQ66" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="JR66" t="n">
+      <c r="JR66" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="JS66" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -56598,8 +56796,11 @@
       <c r="JQ67" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JR67" t="n">
+      <c r="JR67" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="JS67" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -57436,8 +57637,11 @@
       <c r="JQ68" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="JR68" t="n">
+      <c r="JR68" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="JS68" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -58274,7 +58478,10 @@
       <c r="JQ69" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JR69" t="n">
+      <c r="JR69" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JS69" t="n">
         <v>2</v>
       </c>
     </row>
@@ -59112,8 +59319,11 @@
       <c r="JQ70" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="JR70" t="n">
+      <c r="JR70" s="1" t="n">
         <v>23</v>
+      </c>
+      <c r="JS70" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -59950,8 +60160,11 @@
       <c r="JQ71" s="1" t="n">
         <v>48.4</v>
       </c>
-      <c r="JR71" t="n">
+      <c r="JR71" s="1" t="n">
         <v>73.90000000000001</v>
+      </c>
+      <c r="JS71" t="n">
+        <v>61.9</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -60788,8 +61001,11 @@
       <c r="JQ72" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="JR72" t="n">
+      <c r="JR72" s="1" t="n">
         <v>20.47</v>
+      </c>
+      <c r="JS72" t="n">
+        <v>22.85</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -61626,8 +61842,11 @@
       <c r="JQ73" s="1" t="n">
         <v>12.1</v>
       </c>
-      <c r="JR73" t="n">
+      <c r="JR73" s="1" t="n">
         <v>15.13</v>
+      </c>
+      <c r="JS73" t="n">
+        <v>14.14</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -62464,8 +62683,11 @@
       <c r="JQ74" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="JR74" t="n">
+      <c r="JR74" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="JS74" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -63302,8 +63524,11 @@
       <c r="JQ75" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="JR75" t="n">
+      <c r="JR75" s="1" t="n">
         <v>49</v>
+      </c>
+      <c r="JS75" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -64140,8 +64365,11 @@
       <c r="JQ76" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="JR76" t="n">
+      <c r="JR76" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="JS76" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -64978,8 +65206,11 @@
       <c r="JQ77" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="JR77" t="n">
+      <c r="JR77" s="1" t="n">
         <v>51</v>
+      </c>
+      <c r="JS77" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -65816,8 +66047,11 @@
       <c r="JQ78" s="1" t="n">
         <v>1.94</v>
       </c>
-      <c r="JR78" t="n">
+      <c r="JR78" s="1" t="n">
         <v>2.22</v>
+      </c>
+      <c r="JS78" t="n">
+        <v>2.33</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -66654,8 +66888,11 @@
       <c r="JQ79" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JR79" t="n">
+      <c r="JR79" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="JS79" t="n">
+        <v>3.77</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -67492,8 +67729,11 @@
       <c r="JQ80" s="1" t="n">
         <v>46.7</v>
       </c>
-      <c r="JR80" t="n">
+      <c r="JR80" s="1" t="n">
         <v>41.2</v>
+      </c>
+      <c r="JS80" t="n">
+        <v>38.8</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -68330,8 +68570,11 @@
       <c r="JQ81" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="JR81" t="n">
+      <c r="JR81" s="1" t="n">
         <v>33.3</v>
+      </c>
+      <c r="JS81" t="n">
+        <v>26.5</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -69168,8 +69411,11 @@
       <c r="JQ82" s="1" t="n">
         <v>188.6</v>
       </c>
-      <c r="JR82" t="n">
+      <c r="JR82" s="1" t="n">
         <v>187</v>
+      </c>
+      <c r="JS82" t="n">
+        <v>188</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -70006,8 +70252,11 @@
       <c r="JQ83" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="JR83" t="n">
+      <c r="JR83" s="1" t="n">
         <v>87</v>
+      </c>
+      <c r="JS83" t="n">
+        <v>87.7</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -70844,8 +71093,11 @@
       <c r="JQ84" s="1" t="n">
         <v>26.8</v>
       </c>
-      <c r="JR84" t="n">
+      <c r="JR84" s="1" t="n">
         <v>27.49</v>
+      </c>
+      <c r="JS84" t="n">
+        <v>26.41</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -71682,8 +71934,11 @@
       <c r="JQ85" s="1" t="n">
         <v>95.5</v>
       </c>
-      <c r="JR85" t="n">
+      <c r="JR85" s="1" t="n">
         <v>131.7</v>
+      </c>
+      <c r="JS85" t="n">
+        <v>108.8</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -72520,8 +72775,11 @@
       <c r="JQ86" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JR86" t="n">
+      <c r="JR86" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="JS86" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -73358,8 +73616,11 @@
       <c r="JQ87" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="JR87" t="n">
+      <c r="JR87" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="JS87" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -74196,8 +74457,11 @@
       <c r="JQ88" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JR88" t="n">
+      <c r="JR88" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="JS88" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -75034,8 +75298,11 @@
       <c r="JQ89" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="JR89" t="n">
+      <c r="JR89" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="JS89" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -75872,8 +76139,11 @@
       <c r="JQ90" s="1" t="n">
         <v>129</v>
       </c>
-      <c r="JR90" t="n">
+      <c r="JR90" s="1" t="n">
         <v>135</v>
+      </c>
+      <c r="JS90" t="n">
+        <v>124</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -76710,8 +76980,11 @@
       <c r="JQ91" s="1" t="n">
         <v>236</v>
       </c>
-      <c r="JR91" t="n">
+      <c r="JR91" s="1" t="n">
         <v>201</v>
+      </c>
+      <c r="JS91" t="n">
+        <v>161</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -77548,8 +77821,11 @@
       <c r="JQ92" s="1" t="n">
         <v>287</v>
       </c>
-      <c r="JR92" t="n">
+      <c r="JR92" s="1" t="n">
         <v>255</v>
+      </c>
+      <c r="JS92" t="n">
+        <v>215</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -78386,8 +78662,11 @@
       <c r="JQ93" s="1" t="n">
         <v>76.5</v>
       </c>
-      <c r="JR93" t="n">
+      <c r="JR93" s="1" t="n">
         <v>73.3</v>
+      </c>
+      <c r="JS93" t="n">
+        <v>72.40000000000001</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -79224,8 +79503,11 @@
       <c r="JQ94" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="JR94" t="n">
+      <c r="JR94" s="1" t="n">
         <v>49</v>
+      </c>
+      <c r="JS94" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -80062,8 +80344,11 @@
       <c r="JQ95" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JR95" t="n">
+      <c r="JR95" s="1" t="n">
         <v>16</v>
+      </c>
+      <c r="JS95" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -80900,8 +81185,11 @@
       <c r="JQ96" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="JR96" t="n">
+      <c r="JR96" s="1" t="n">
         <v>16</v>
+      </c>
+      <c r="JS96" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -81738,8 +82026,11 @@
       <c r="JQ97" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="JR97" t="n">
+      <c r="JR97" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="JS97" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -82576,8 +82867,11 @@
       <c r="JQ98" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="JR98" t="n">
+      <c r="JR98" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="JS98" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -83414,8 +83708,11 @@
       <c r="JQ99" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="JR99" t="n">
+      <c r="JR99" s="1" t="n">
         <v>52</v>
+      </c>
+      <c r="JS99" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -84252,8 +84549,11 @@
       <c r="JQ100" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="JR100" t="n">
+      <c r="JR100" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="JS100" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -85090,8 +85390,11 @@
       <c r="JQ101" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JR101" t="n">
+      <c r="JR101" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="JS101" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -85928,8 +86231,11 @@
       <c r="JQ102" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="JR102" t="n">
+      <c r="JR102" s="1" t="n">
         <v>70.59999999999999</v>
+      </c>
+      <c r="JS102" t="n">
+        <v>76.90000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023 round 5 predictions done
</commit_message>
<xml_diff>
--- a/AFL_ML/Data/Adelaide_stats.xlsx
+++ b/AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:JS102"/>
+  <dimension ref="A1:JT102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1293,8 +1293,11 @@
       <c r="JR1" s="1" t="n">
         <v>10763</v>
       </c>
-      <c r="JS1" t="n">
+      <c r="JS1" s="1" t="n">
         <v>10774</v>
+      </c>
+      <c r="JT1" t="n">
+        <v>10780</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -2134,7 +2137,10 @@
       <c r="JR2" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="JS2" t="n">
+      <c r="JS2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="JT2" t="n">
         <v>2023</v>
       </c>
     </row>
@@ -2975,8 +2981,11 @@
       <c r="JR3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="JS3" t="n">
+      <c r="JS3" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="JT3" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3816,8 +3825,11 @@
       <c r="JR4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JS4" t="n">
+      <c r="JS4" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="JT4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -4657,8 +4669,11 @@
       <c r="JR5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JS5" t="n">
+      <c r="JS5" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="JT5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="2">
@@ -5498,8 +5513,11 @@
       <c r="JR6" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="JS6" t="n">
+      <c r="JS6" s="1" t="n">
         <v>117</v>
+      </c>
+      <c r="JT6" t="n">
+        <v>111</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -6339,8 +6357,11 @@
       <c r="JR7" s="1" t="n">
         <v>108</v>
       </c>
-      <c r="JS7" t="n">
+      <c r="JS7" s="1" t="n">
         <v>86</v>
+      </c>
+      <c r="JT7" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -7180,8 +7201,11 @@
       <c r="JR8" s="1" t="n">
         <v>-32</v>
       </c>
-      <c r="JS8" t="n">
+      <c r="JS8" s="1" t="n">
         <v>31</v>
+      </c>
+      <c r="JT8" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -8021,7 +8045,10 @@
       <c r="JR9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JS9" t="n">
+      <c r="JS9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JT9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -8862,8 +8889,11 @@
       <c r="JR10" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="JS10" t="n">
+      <c r="JS10" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="JT10" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -9703,8 +9733,11 @@
       <c r="JR11" s="1" t="n">
         <v>216</v>
       </c>
-      <c r="JS11" t="n">
+      <c r="JS11" s="1" t="n">
         <v>212</v>
+      </c>
+      <c r="JT11" t="n">
+        <v>222</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -10544,8 +10577,11 @@
       <c r="JR12" s="1" t="n">
         <v>142</v>
       </c>
-      <c r="JS12" t="n">
+      <c r="JS12" s="1" t="n">
         <v>120</v>
+      </c>
+      <c r="JT12" t="n">
+        <v>158</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -11385,8 +11421,11 @@
       <c r="JR13" s="1" t="n">
         <v>358</v>
       </c>
-      <c r="JS13" t="n">
+      <c r="JS13" s="1" t="n">
         <v>332</v>
+      </c>
+      <c r="JT13" t="n">
+        <v>380</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -12226,8 +12265,11 @@
       <c r="JR14" s="1" t="n">
         <v>1.52</v>
       </c>
-      <c r="JS14" t="n">
+      <c r="JS14" s="1" t="n">
         <v>1.77</v>
+      </c>
+      <c r="JT14" t="n">
+        <v>1.41</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -13067,8 +13109,11 @@
       <c r="JR15" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="JS15" t="n">
+      <c r="JS15" s="1" t="n">
         <v>88</v>
+      </c>
+      <c r="JT15" t="n">
+        <v>87</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -13908,8 +13953,11 @@
       <c r="JR16" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="JS16" t="n">
+      <c r="JS16" s="1" t="n">
         <v>59</v>
+      </c>
+      <c r="JT16" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -14749,8 +14797,11 @@
       <c r="JR17" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="JS17" t="n">
+      <c r="JS17" s="1" t="n">
         <v>45</v>
+      </c>
+      <c r="JT17" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -15590,7 +15641,10 @@
       <c r="JR18" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="JS18" t="n">
+      <c r="JS18" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JT18" t="n">
         <v>22</v>
       </c>
     </row>
@@ -16431,8 +16485,11 @@
       <c r="JR19" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="JS19" t="n">
+      <c r="JS19" s="1" t="n">
         <v>29</v>
+      </c>
+      <c r="JT19" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -17272,8 +17329,11 @@
       <c r="JR20" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="JS20" t="n">
+      <c r="JS20" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="JT20" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -18113,8 +18173,11 @@
       <c r="JR21" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JS21" t="n">
+      <c r="JS21" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="JT21" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -18954,8 +19017,11 @@
       <c r="JR22" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="JS22" t="n">
+      <c r="JS22" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="JT22" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -19795,8 +19861,11 @@
       <c r="JR23" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JS23" t="n">
+      <c r="JS23" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="JT23" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -20636,8 +20705,11 @@
       <c r="JR24" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="JS24" t="n">
+      <c r="JS24" s="1" t="n">
         <v>27</v>
+      </c>
+      <c r="JT24" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -21477,8 +21549,11 @@
       <c r="JR25" s="1" t="n">
         <v>38.5</v>
       </c>
-      <c r="JS25" t="n">
+      <c r="JS25" s="1" t="n">
         <v>66.7</v>
+      </c>
+      <c r="JT25" t="n">
+        <v>65.40000000000001</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -22318,8 +22393,11 @@
       <c r="JR26" s="1" t="n">
         <v>35.8</v>
       </c>
-      <c r="JS26" t="n">
+      <c r="JS26" s="1" t="n">
         <v>18.44</v>
+      </c>
+      <c r="JT26" t="n">
+        <v>22.35</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -23159,8 +23237,11 @@
       <c r="JR27" s="1" t="n">
         <v>13.77</v>
       </c>
-      <c r="JS27" t="n">
+      <c r="JS27" s="1" t="n">
         <v>12.3</v>
+      </c>
+      <c r="JT27" t="n">
+        <v>14.62</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -24000,8 +24081,11 @@
       <c r="JR28" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="JS28" t="n">
+      <c r="JS28" s="1" t="n">
         <v>39</v>
+      </c>
+      <c r="JT28" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -24841,8 +24925,11 @@
       <c r="JR29" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="JS29" t="n">
+      <c r="JS29" s="1" t="n">
         <v>60</v>
+      </c>
+      <c r="JT29" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -25682,8 +25769,11 @@
       <c r="JR30" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="JS30" t="n">
+      <c r="JS30" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="JT30" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -26523,8 +26613,11 @@
       <c r="JR31" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="JS31" t="n">
+      <c r="JS31" s="1" t="n">
         <v>59</v>
+      </c>
+      <c r="JT31" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -27364,8 +27457,11 @@
       <c r="JR32" s="1" t="n">
         <v>2.04</v>
       </c>
-      <c r="JS32" t="n">
+      <c r="JS32" s="1" t="n">
         <v>2.19</v>
+      </c>
+      <c r="JT32" t="n">
+        <v>1.96</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -28205,8 +28301,11 @@
       <c r="JR33" s="1" t="n">
         <v>5.3</v>
       </c>
-      <c r="JS33" t="n">
+      <c r="JS33" s="1" t="n">
         <v>3.28</v>
+      </c>
+      <c r="JT33" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -29046,8 +29145,11 @@
       <c r="JR34" s="1" t="n">
         <v>43.4</v>
       </c>
-      <c r="JS34" t="n">
+      <c r="JS34" s="1" t="n">
         <v>44.1</v>
+      </c>
+      <c r="JT34" t="n">
+        <v>47.1</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -29887,8 +29989,11 @@
       <c r="JR35" s="1" t="n">
         <v>18.9</v>
       </c>
-      <c r="JS35" t="n">
+      <c r="JS35" s="1" t="n">
         <v>30.5</v>
+      </c>
+      <c r="JT35" t="n">
+        <v>33.3</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -30728,8 +30833,11 @@
       <c r="JR36" s="1" t="n">
         <v>187.3</v>
       </c>
-      <c r="JS36" t="n">
+      <c r="JS36" s="1" t="n">
         <v>187.3</v>
+      </c>
+      <c r="JT36" t="n">
+        <v>187.1</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -31569,8 +31677,11 @@
       <c r="JR37" s="1" t="n">
         <v>87.59999999999999</v>
       </c>
-      <c r="JS37" t="n">
+      <c r="JS37" s="1" t="n">
         <v>87.5</v>
+      </c>
+      <c r="JT37" t="n">
+        <v>87</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -32410,8 +32521,11 @@
       <c r="JR38" s="1" t="n">
         <v>24.49</v>
       </c>
-      <c r="JS38" t="n">
+      <c r="JS38" s="1" t="n">
         <v>24.58</v>
+      </c>
+      <c r="JT38" t="n">
+        <v>24.74</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -33251,8 +33365,11 @@
       <c r="JR39" s="1" t="n">
         <v>74.90000000000001</v>
       </c>
-      <c r="JS39" t="n">
+      <c r="JS39" s="1" t="n">
         <v>77</v>
+      </c>
+      <c r="JT39" t="n">
+        <v>80.2</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -34092,8 +34209,11 @@
       <c r="JR40" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="JS40" t="n">
+      <c r="JS40" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="JT40" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="2">
@@ -34933,8 +35053,11 @@
       <c r="JR41" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JS41" t="n">
+      <c r="JS41" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="JT41" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="2">
@@ -35774,7 +35897,10 @@
       <c r="JR42" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JS42" t="n">
+      <c r="JS42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JT42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -36615,7 +36741,10 @@
       <c r="JR43" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JS43" t="n">
+      <c r="JS43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JT43" t="n">
         <v>4</v>
       </c>
     </row>
@@ -37456,8 +37585,11 @@
       <c r="JR44" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="JS44" t="n">
+      <c r="JS44" s="1" t="n">
         <v>146</v>
+      </c>
+      <c r="JT44" t="n">
+        <v>151</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -38297,8 +38429,11 @@
       <c r="JR45" s="1" t="n">
         <v>213</v>
       </c>
-      <c r="JS45" t="n">
+      <c r="JS45" s="1" t="n">
         <v>183</v>
+      </c>
+      <c r="JT45" t="n">
+        <v>224</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -39138,8 +39273,11 @@
       <c r="JR46" s="1" t="n">
         <v>253</v>
       </c>
-      <c r="JS46" t="n">
+      <c r="JS46" s="1" t="n">
         <v>251</v>
+      </c>
+      <c r="JT46" t="n">
+        <v>276</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -39979,8 +40117,11 @@
       <c r="JR47" s="1" t="n">
         <v>70.7</v>
       </c>
-      <c r="JS47" t="n">
+      <c r="JS47" s="1" t="n">
         <v>75.59999999999999</v>
+      </c>
+      <c r="JT47" t="n">
+        <v>72.59999999999999</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -40820,8 +40961,11 @@
       <c r="JR48" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="JS48" t="n">
+      <c r="JS48" s="1" t="n">
         <v>60</v>
+      </c>
+      <c r="JT48" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -41661,8 +41805,11 @@
       <c r="JR49" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="JS49" t="n">
+      <c r="JS49" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="JT49" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -42502,8 +42649,11 @@
       <c r="JR50" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="JS50" t="n">
+      <c r="JS50" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="JT50" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -43343,8 +43493,11 @@
       <c r="JR51" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="JS51" t="n">
+      <c r="JS51" s="1" t="n">
         <v>39</v>
+      </c>
+      <c r="JT51" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -44184,8 +44337,11 @@
       <c r="JR52" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="JS52" t="n">
+      <c r="JS52" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="JT52" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -45025,8 +45181,11 @@
       <c r="JR53" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="JS53" t="n">
+      <c r="JS53" s="1" t="n">
         <v>49</v>
+      </c>
+      <c r="JT53" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -45866,8 +46025,11 @@
       <c r="JR54" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JS54" t="n">
+      <c r="JS54" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="JT54" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -46707,8 +46869,11 @@
       <c r="JR55" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JS55" t="n">
+      <c r="JS55" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="JT55" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -47548,8 +47713,11 @@
       <c r="JR56" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="JS56" t="n">
+      <c r="JS56" s="1" t="n">
         <v>72.2</v>
+      </c>
+      <c r="JT56" t="n">
+        <v>70.59999999999999</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -48389,8 +48557,11 @@
       <c r="JR57" s="1" t="n">
         <v>209</v>
       </c>
-      <c r="JS57" t="n">
+      <c r="JS57" s="1" t="n">
         <v>188</v>
+      </c>
+      <c r="JT57" t="n">
+        <v>179</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -49230,8 +49401,11 @@
       <c r="JR58" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="JS58" t="n">
+      <c r="JS58" s="1" t="n">
         <v>109</v>
+      </c>
+      <c r="JT58" t="n">
+        <v>155</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -50071,8 +50245,11 @@
       <c r="JR59" s="1" t="n">
         <v>348</v>
       </c>
-      <c r="JS59" t="n">
+      <c r="JS59" s="1" t="n">
         <v>297</v>
+      </c>
+      <c r="JT59" t="n">
+        <v>334</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -50912,8 +51089,11 @@
       <c r="JR60" s="1" t="n">
         <v>1.5</v>
       </c>
-      <c r="JS60" t="n">
+      <c r="JS60" s="1" t="n">
         <v>1.72</v>
+      </c>
+      <c r="JT60" t="n">
+        <v>1.15</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -51753,8 +51933,11 @@
       <c r="JR61" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="JS61" t="n">
+      <c r="JS61" s="1" t="n">
         <v>63</v>
+      </c>
+      <c r="JT61" t="n">
+        <v>61</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -52594,8 +52777,11 @@
       <c r="JR62" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="JS62" t="n">
+      <c r="JS62" s="1" t="n">
         <v>76</v>
+      </c>
+      <c r="JT62" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -53435,8 +53621,11 @@
       <c r="JR63" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="JS63" t="n">
+      <c r="JS63" s="1" t="n">
         <v>38</v>
+      </c>
+      <c r="JT63" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -54276,8 +54465,11 @@
       <c r="JR64" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="JS64" t="n">
+      <c r="JS64" s="1" t="n">
         <v>29</v>
+      </c>
+      <c r="JT64" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -55117,8 +55309,11 @@
       <c r="JR65" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="JS65" t="n">
+      <c r="JS65" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="JT65" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -55958,8 +56153,11 @@
       <c r="JR66" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="JS66" t="n">
+      <c r="JS66" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="JT66" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -56799,8 +56997,11 @@
       <c r="JR67" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="JS67" t="n">
+      <c r="JS67" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="JT67" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -57640,8 +57841,11 @@
       <c r="JR68" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JS68" t="n">
+      <c r="JS68" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="JT68" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -58481,8 +58685,11 @@
       <c r="JR69" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="JS69" t="n">
+      <c r="JS69" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="JT69" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -59322,8 +59529,11 @@
       <c r="JR70" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="JS70" t="n">
+      <c r="JS70" s="1" t="n">
         <v>21</v>
+      </c>
+      <c r="JT70" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -60163,8 +60373,11 @@
       <c r="JR71" s="1" t="n">
         <v>73.90000000000001</v>
       </c>
-      <c r="JS71" t="n">
+      <c r="JS71" s="1" t="n">
         <v>61.9</v>
+      </c>
+      <c r="JT71" t="n">
+        <v>45.5</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -61004,8 +61217,11 @@
       <c r="JR72" s="1" t="n">
         <v>20.47</v>
       </c>
-      <c r="JS72" t="n">
+      <c r="JS72" s="1" t="n">
         <v>22.85</v>
+      </c>
+      <c r="JT72" t="n">
+        <v>33.4</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -61845,8 +62061,11 @@
       <c r="JR73" s="1" t="n">
         <v>15.13</v>
       </c>
-      <c r="JS73" t="n">
+      <c r="JS73" s="1" t="n">
         <v>14.14</v>
+      </c>
+      <c r="JT73" t="n">
+        <v>15.18</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -62686,8 +62905,11 @@
       <c r="JR74" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="JS74" t="n">
+      <c r="JS74" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="JT74" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -63527,8 +63749,11 @@
       <c r="JR75" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="JS75" t="n">
+      <c r="JS75" s="1" t="n">
         <v>59</v>
+      </c>
+      <c r="JT75" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -64368,8 +64593,11 @@
       <c r="JR76" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="JS76" t="n">
+      <c r="JS76" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="JT76" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -65209,8 +65437,11 @@
       <c r="JR77" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="JS77" t="n">
+      <c r="JS77" s="1" t="n">
         <v>49</v>
+      </c>
+      <c r="JT77" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -66050,8 +66281,11 @@
       <c r="JR78" s="1" t="n">
         <v>2.22</v>
       </c>
-      <c r="JS78" t="n">
+      <c r="JS78" s="1" t="n">
         <v>2.33</v>
+      </c>
+      <c r="JT78" t="n">
+        <v>2.32</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -66891,8 +67125,11 @@
       <c r="JR79" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JS79" t="n">
+      <c r="JS79" s="1" t="n">
         <v>3.77</v>
+      </c>
+      <c r="JT79" t="n">
+        <v>5.1</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -67732,8 +67969,11 @@
       <c r="JR80" s="1" t="n">
         <v>41.2</v>
       </c>
-      <c r="JS80" t="n">
+      <c r="JS80" s="1" t="n">
         <v>38.8</v>
+      </c>
+      <c r="JT80" t="n">
+        <v>33.3</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -68573,8 +68813,11 @@
       <c r="JR81" s="1" t="n">
         <v>33.3</v>
       </c>
-      <c r="JS81" t="n">
+      <c r="JS81" s="1" t="n">
         <v>26.5</v>
+      </c>
+      <c r="JT81" t="n">
+        <v>19.6</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -69414,7 +69657,10 @@
       <c r="JR82" s="1" t="n">
         <v>187</v>
       </c>
-      <c r="JS82" t="n">
+      <c r="JS82" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="JT82" t="n">
         <v>188</v>
       </c>
     </row>
@@ -70255,8 +70501,11 @@
       <c r="JR83" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="JS83" t="n">
+      <c r="JS83" s="1" t="n">
         <v>87.7</v>
+      </c>
+      <c r="JT83" t="n">
+        <v>87</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -71096,8 +71345,11 @@
       <c r="JR84" s="1" t="n">
         <v>27.49</v>
       </c>
-      <c r="JS84" t="n">
+      <c r="JS84" s="1" t="n">
         <v>26.41</v>
+      </c>
+      <c r="JT84" t="n">
+        <v>24.91</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -71937,8 +72189,11 @@
       <c r="JR85" s="1" t="n">
         <v>131.7</v>
       </c>
-      <c r="JS85" t="n">
+      <c r="JS85" s="1" t="n">
         <v>108.8</v>
+      </c>
+      <c r="JT85" t="n">
+        <v>79.3</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -72778,8 +73033,11 @@
       <c r="JR86" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JS86" t="n">
+      <c r="JS86" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="JT86" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -73619,7 +73877,10 @@
       <c r="JR87" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="JS87" t="n">
+      <c r="JS87" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JT87" t="n">
         <v>10</v>
       </c>
     </row>
@@ -74460,7 +74721,10 @@
       <c r="JR88" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JS88" t="n">
+      <c r="JS88" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JT88" t="n">
         <v>5</v>
       </c>
     </row>
@@ -75301,8 +75565,11 @@
       <c r="JR89" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JS89" t="n">
+      <c r="JS89" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="JT89" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -76142,8 +76409,11 @@
       <c r="JR90" s="1" t="n">
         <v>135</v>
       </c>
-      <c r="JS90" t="n">
+      <c r="JS90" s="1" t="n">
         <v>124</v>
+      </c>
+      <c r="JT90" t="n">
+        <v>137</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -76983,8 +77253,11 @@
       <c r="JR91" s="1" t="n">
         <v>201</v>
       </c>
-      <c r="JS91" t="n">
+      <c r="JS91" s="1" t="n">
         <v>161</v>
+      </c>
+      <c r="JT91" t="n">
+        <v>189</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -77824,8 +78097,11 @@
       <c r="JR92" s="1" t="n">
         <v>255</v>
       </c>
-      <c r="JS92" t="n">
+      <c r="JS92" s="1" t="n">
         <v>215</v>
+      </c>
+      <c r="JT92" t="n">
+        <v>239</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -78665,8 +78941,11 @@
       <c r="JR93" s="1" t="n">
         <v>73.3</v>
       </c>
-      <c r="JS93" t="n">
+      <c r="JS93" s="1" t="n">
         <v>72.40000000000001</v>
+      </c>
+      <c r="JT93" t="n">
+        <v>71.59999999999999</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -79506,8 +79785,11 @@
       <c r="JR94" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="JS94" t="n">
+      <c r="JS94" s="1" t="n">
         <v>59</v>
+      </c>
+      <c r="JT94" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -80347,8 +80629,11 @@
       <c r="JR95" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="JS95" t="n">
+      <c r="JS95" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="JT95" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -81188,8 +81473,11 @@
       <c r="JR96" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="JS96" t="n">
+      <c r="JS96" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="JT96" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -82029,8 +82317,11 @@
       <c r="JR97" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="JS97" t="n">
+      <c r="JS97" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="JT97" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -82870,8 +83161,11 @@
       <c r="JR98" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="JS98" t="n">
+      <c r="JS98" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="JT98" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -83711,8 +84005,11 @@
       <c r="JR99" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="JS99" t="n">
+      <c r="JS99" s="1" t="n">
         <v>51</v>
+      </c>
+      <c r="JT99" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -84552,8 +84849,11 @@
       <c r="JR100" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="JS100" t="n">
+      <c r="JS100" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="JT100" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -85393,8 +85693,11 @@
       <c r="JR101" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="JS101" t="n">
+      <c r="JS101" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="JT101" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -86234,8 +86537,11 @@
       <c r="JR102" s="1" t="n">
         <v>70.59999999999999</v>
       </c>
-      <c r="JS102" t="n">
+      <c r="JS102" s="1" t="n">
         <v>76.90000000000001</v>
+      </c>
+      <c r="JT102" t="n">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with round 5 2023 results
</commit_message>
<xml_diff>
--- a/AFL_ML/Data/Adelaide_stats.xlsx
+++ b/AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:JT102"/>
+  <dimension ref="A1:JV102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1296,8 +1296,14 @@
       <c r="JS1" s="1" t="n">
         <v>10774</v>
       </c>
-      <c r="JT1" t="n">
+      <c r="JT1" s="1" t="n">
         <v>10780</v>
+      </c>
+      <c r="JU1" s="1" t="n">
+        <v>10787</v>
+      </c>
+      <c r="JV1" t="n">
+        <v>10787</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -2140,7 +2146,13 @@
       <c r="JS2" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="JT2" t="n">
+      <c r="JT2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="JU2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="JV2" t="n">
         <v>2023</v>
       </c>
     </row>
@@ -2984,8 +2996,14 @@
       <c r="JS3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JT3" t="n">
+      <c r="JT3" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="JU3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JV3" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3828,7 +3846,13 @@
       <c r="JS4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JT4" t="n">
+      <c r="JT4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JU4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JV4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4672,7 +4696,13 @@
       <c r="JS5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JT5" t="n">
+      <c r="JT5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JU5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JV5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5516,8 +5546,14 @@
       <c r="JS6" s="1" t="n">
         <v>117</v>
       </c>
-      <c r="JT6" t="n">
+      <c r="JT6" s="1" t="n">
         <v>111</v>
+      </c>
+      <c r="JU6" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="JV6" t="n">
+        <v>118</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -6360,8 +6396,14 @@
       <c r="JS7" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="JT7" t="n">
+      <c r="JT7" s="1" t="n">
         <v>72</v>
+      </c>
+      <c r="JU7" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="JV7" t="n">
+        <v>62</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -7204,8 +7246,14 @@
       <c r="JS8" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="JT8" t="n">
+      <c r="JT8" s="1" t="n">
         <v>39</v>
+      </c>
+      <c r="JU8" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="JV8" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -8048,7 +8096,13 @@
       <c r="JS9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JT9" t="n">
+      <c r="JT9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JU9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JV9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -8892,8 +8946,14 @@
       <c r="JS10" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="JT10" t="n">
+      <c r="JT10" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="JU10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JV10" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -9736,8 +9796,14 @@
       <c r="JS11" s="1" t="n">
         <v>212</v>
       </c>
-      <c r="JT11" t="n">
+      <c r="JT11" s="1" t="n">
         <v>222</v>
+      </c>
+      <c r="JU11" s="1" t="n">
+        <v>242</v>
+      </c>
+      <c r="JV11" t="n">
+        <v>242</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -10580,8 +10646,14 @@
       <c r="JS12" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="JT12" t="n">
+      <c r="JT12" s="1" t="n">
         <v>158</v>
+      </c>
+      <c r="JU12" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="JV12" t="n">
+        <v>156</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -11424,8 +11496,14 @@
       <c r="JS13" s="1" t="n">
         <v>332</v>
       </c>
-      <c r="JT13" t="n">
+      <c r="JT13" s="1" t="n">
         <v>380</v>
+      </c>
+      <c r="JU13" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="JV13" t="n">
+        <v>398</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -12268,8 +12346,14 @@
       <c r="JS14" s="1" t="n">
         <v>1.77</v>
       </c>
-      <c r="JT14" t="n">
+      <c r="JT14" s="1" t="n">
         <v>1.41</v>
+      </c>
+      <c r="JU14" s="1" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="JV14" t="n">
+        <v>1.55</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -13112,8 +13196,14 @@
       <c r="JS15" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="JT15" t="n">
+      <c r="JT15" s="1" t="n">
         <v>87</v>
+      </c>
+      <c r="JU15" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="JV15" t="n">
+        <v>116</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -13956,8 +14046,14 @@
       <c r="JS16" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="JT16" t="n">
+      <c r="JT16" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="JU16" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="JV16" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -14800,8 +14896,14 @@
       <c r="JS17" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="JT17" t="n">
+      <c r="JT17" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="JU17" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="JV17" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -15644,7 +15746,13 @@
       <c r="JS18" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="JT18" t="n">
+      <c r="JT18" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JU18" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JV18" t="n">
         <v>22</v>
       </c>
     </row>
@@ -16488,8 +16596,14 @@
       <c r="JS19" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="JT19" t="n">
+      <c r="JT19" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="JU19" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JV19" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -17332,8 +17446,14 @@
       <c r="JS20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="JT20" t="n">
+      <c r="JT20" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="JU20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="JV20" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -18176,8 +18296,14 @@
       <c r="JS21" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="JT21" t="n">
+      <c r="JT21" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="JU21" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="JV21" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -19020,8 +19146,14 @@
       <c r="JS22" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JT22" t="n">
+      <c r="JT22" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="JU22" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JV22" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -19864,8 +19996,14 @@
       <c r="JS23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JT23" t="n">
+      <c r="JT23" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="JU23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JV23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -20708,8 +20846,14 @@
       <c r="JS24" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="JT24" t="n">
+      <c r="JT24" s="1" t="n">
         <v>26</v>
+      </c>
+      <c r="JU24" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="JV24" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -21552,8 +21696,14 @@
       <c r="JS25" s="1" t="n">
         <v>66.7</v>
       </c>
-      <c r="JT25" t="n">
+      <c r="JT25" s="1" t="n">
         <v>65.40000000000001</v>
+      </c>
+      <c r="JU25" s="1" t="n">
+        <v>64.3</v>
+      </c>
+      <c r="JV25" t="n">
+        <v>64.3</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -22396,8 +22546,14 @@
       <c r="JS26" s="1" t="n">
         <v>18.44</v>
       </c>
-      <c r="JT26" t="n">
+      <c r="JT26" s="1" t="n">
         <v>22.35</v>
+      </c>
+      <c r="JU26" s="1" t="n">
+        <v>22.11</v>
+      </c>
+      <c r="JV26" t="n">
+        <v>22.11</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -23240,8 +23396,14 @@
       <c r="JS27" s="1" t="n">
         <v>12.3</v>
       </c>
-      <c r="JT27" t="n">
+      <c r="JT27" s="1" t="n">
         <v>14.62</v>
+      </c>
+      <c r="JU27" s="1" t="n">
+        <v>14.21</v>
+      </c>
+      <c r="JV27" t="n">
+        <v>14.21</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -24084,8 +24246,14 @@
       <c r="JS28" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="JT28" t="n">
+      <c r="JT28" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="JU28" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="JV28" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -24928,8 +25096,14 @@
       <c r="JS29" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="JT29" t="n">
+      <c r="JT29" s="1" t="n">
         <v>63</v>
+      </c>
+      <c r="JU29" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="JV29" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -25772,8 +25946,14 @@
       <c r="JS30" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="JT30" t="n">
+      <c r="JT30" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="JU30" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="JV30" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -26616,7 +26796,13 @@
       <c r="JS31" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="JT31" t="n">
+      <c r="JT31" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JU31" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JV31" t="n">
         <v>51</v>
       </c>
     </row>
@@ -27460,8 +27646,14 @@
       <c r="JS32" s="1" t="n">
         <v>2.19</v>
       </c>
-      <c r="JT32" t="n">
+      <c r="JT32" s="1" t="n">
         <v>1.96</v>
+      </c>
+      <c r="JU32" s="1" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="JV32" t="n">
+        <v>1.82</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -28304,8 +28496,14 @@
       <c r="JS33" s="1" t="n">
         <v>3.28</v>
       </c>
-      <c r="JT33" t="n">
+      <c r="JT33" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="JU33" s="1" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="JV33" t="n">
+        <v>2.83</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -29148,8 +29346,14 @@
       <c r="JS34" s="1" t="n">
         <v>44.1</v>
       </c>
-      <c r="JT34" t="n">
+      <c r="JT34" s="1" t="n">
         <v>47.1</v>
+      </c>
+      <c r="JU34" s="1" t="n">
+        <v>54.9</v>
+      </c>
+      <c r="JV34" t="n">
+        <v>54.9</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -29992,8 +30196,14 @@
       <c r="JS35" s="1" t="n">
         <v>30.5</v>
       </c>
-      <c r="JT35" t="n">
+      <c r="JT35" s="1" t="n">
         <v>33.3</v>
+      </c>
+      <c r="JU35" s="1" t="n">
+        <v>35.3</v>
+      </c>
+      <c r="JV35" t="n">
+        <v>35.3</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -30836,8 +31046,14 @@
       <c r="JS36" s="1" t="n">
         <v>187.3</v>
       </c>
-      <c r="JT36" t="n">
+      <c r="JT36" s="1" t="n">
         <v>187.1</v>
+      </c>
+      <c r="JU36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="JV36" t="n">
+        <v>187.3</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -31680,8 +31896,14 @@
       <c r="JS37" s="1" t="n">
         <v>87.5</v>
       </c>
-      <c r="JT37" t="n">
+      <c r="JT37" s="1" t="n">
         <v>87</v>
+      </c>
+      <c r="JU37" s="1" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="JV37" t="n">
+        <v>87.59999999999999</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -32524,7 +32746,13 @@
       <c r="JS38" s="1" t="n">
         <v>24.58</v>
       </c>
-      <c r="JT38" t="n">
+      <c r="JT38" s="1" t="n">
+        <v>24.74</v>
+      </c>
+      <c r="JU38" s="1" t="n">
+        <v>24.74</v>
+      </c>
+      <c r="JV38" t="n">
         <v>24.74</v>
       </c>
     </row>
@@ -33368,8 +33596,14 @@
       <c r="JS39" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="JT39" t="n">
+      <c r="JT39" s="1" t="n">
         <v>80.2</v>
+      </c>
+      <c r="JU39" s="1" t="n">
+        <v>81.59999999999999</v>
+      </c>
+      <c r="JV39" t="n">
+        <v>81.59999999999999</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -34212,8 +34446,14 @@
       <c r="JS40" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="JT40" t="n">
+      <c r="JT40" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="JU40" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JV40" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="2">
@@ -35056,8 +35296,14 @@
       <c r="JS41" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JT41" t="n">
+      <c r="JT41" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="JU41" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JV41" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="2">
@@ -35900,7 +36146,13 @@
       <c r="JS42" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JT42" t="n">
+      <c r="JT42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JU42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JV42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -36744,7 +36996,13 @@
       <c r="JS43" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JT43" t="n">
+      <c r="JT43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JU43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JV43" t="n">
         <v>4</v>
       </c>
     </row>
@@ -37588,8 +37846,14 @@
       <c r="JS44" s="1" t="n">
         <v>146</v>
       </c>
-      <c r="JT44" t="n">
+      <c r="JT44" s="1" t="n">
         <v>151</v>
+      </c>
+      <c r="JU44" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="JV44" t="n">
+        <v>156</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -38432,8 +38696,14 @@
       <c r="JS45" s="1" t="n">
         <v>183</v>
       </c>
-      <c r="JT45" t="n">
+      <c r="JT45" s="1" t="n">
         <v>224</v>
+      </c>
+      <c r="JU45" s="1" t="n">
+        <v>240</v>
+      </c>
+      <c r="JV45" t="n">
+        <v>240</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -39276,8 +39546,14 @@
       <c r="JS46" s="1" t="n">
         <v>251</v>
       </c>
-      <c r="JT46" t="n">
+      <c r="JT46" s="1" t="n">
         <v>276</v>
+      </c>
+      <c r="JU46" s="1" t="n">
+        <v>302</v>
+      </c>
+      <c r="JV46" t="n">
+        <v>302</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -40120,8 +40396,14 @@
       <c r="JS47" s="1" t="n">
         <v>75.59999999999999</v>
       </c>
-      <c r="JT47" t="n">
+      <c r="JT47" s="1" t="n">
         <v>72.59999999999999</v>
+      </c>
+      <c r="JU47" s="1" t="n">
+        <v>75.90000000000001</v>
+      </c>
+      <c r="JV47" t="n">
+        <v>75.90000000000001</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -40964,8 +41246,14 @@
       <c r="JS48" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="JT48" t="n">
+      <c r="JT48" s="1" t="n">
         <v>63</v>
+      </c>
+      <c r="JU48" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="JV48" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -41808,8 +42096,14 @@
       <c r="JS49" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JT49" t="n">
+      <c r="JT49" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="JU49" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="JV49" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -42652,8 +42946,14 @@
       <c r="JS50" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="JT50" t="n">
+      <c r="JT50" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="JU50" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="JV50" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -43496,8 +43796,14 @@
       <c r="JS51" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="JT51" t="n">
+      <c r="JT51" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="JU51" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="JV51" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -44340,8 +44646,14 @@
       <c r="JS52" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="JT52" t="n">
+      <c r="JT52" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="JU52" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="JV52" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -45184,8 +45496,14 @@
       <c r="JS53" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="JT53" t="n">
+      <c r="JT53" s="1" t="n">
         <v>53</v>
+      </c>
+      <c r="JU53" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="JV53" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -46028,7 +46346,13 @@
       <c r="JS54" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JT54" t="n">
+      <c r="JT54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JU54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JV54" t="n">
         <v>3</v>
       </c>
     </row>
@@ -46872,8 +47196,14 @@
       <c r="JS55" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="JT55" t="n">
+      <c r="JT55" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="JU55" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="JV55" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -47716,8 +48046,14 @@
       <c r="JS56" s="1" t="n">
         <v>72.2</v>
       </c>
-      <c r="JT56" t="n">
+      <c r="JT56" s="1" t="n">
         <v>70.59999999999999</v>
+      </c>
+      <c r="JU56" s="1" t="n">
+        <v>83.3</v>
+      </c>
+      <c r="JV56" t="n">
+        <v>83.3</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -48560,8 +48896,14 @@
       <c r="JS57" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="JT57" t="n">
+      <c r="JT57" s="1" t="n">
         <v>179</v>
+      </c>
+      <c r="JU57" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="JV57" t="n">
+        <v>183</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -49404,8 +49746,14 @@
       <c r="JS58" s="1" t="n">
         <v>109</v>
       </c>
-      <c r="JT58" t="n">
+      <c r="JT58" s="1" t="n">
         <v>155</v>
+      </c>
+      <c r="JU58" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="JV58" t="n">
+        <v>137</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -50248,8 +50596,14 @@
       <c r="JS59" s="1" t="n">
         <v>297</v>
       </c>
-      <c r="JT59" t="n">
+      <c r="JT59" s="1" t="n">
         <v>334</v>
+      </c>
+      <c r="JU59" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="JV59" t="n">
+        <v>320</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -51092,8 +51446,14 @@
       <c r="JS60" s="1" t="n">
         <v>1.72</v>
       </c>
-      <c r="JT60" t="n">
+      <c r="JT60" s="1" t="n">
         <v>1.15</v>
+      </c>
+      <c r="JU60" s="1" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="JV60" t="n">
+        <v>1.34</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -51936,8 +52296,14 @@
       <c r="JS61" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="JT61" t="n">
+      <c r="JT61" s="1" t="n">
         <v>61</v>
+      </c>
+      <c r="JU61" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="JV61" t="n">
+        <v>71</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -52780,8 +53146,14 @@
       <c r="JS62" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="JT62" t="n">
+      <c r="JT62" s="1" t="n">
         <v>67</v>
+      </c>
+      <c r="JU62" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="JV62" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -53624,8 +53996,14 @@
       <c r="JS63" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="JT63" t="n">
+      <c r="JT63" s="1" t="n">
         <v>46</v>
+      </c>
+      <c r="JU63" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="JV63" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -54468,8 +54846,14 @@
       <c r="JS64" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="JT64" t="n">
+      <c r="JT64" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="JU64" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JV64" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -55312,8 +55696,14 @@
       <c r="JS65" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="JT65" t="n">
+      <c r="JT65" s="1" t="n">
         <v>21</v>
+      </c>
+      <c r="JU65" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JV65" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -56156,8 +56546,14 @@
       <c r="JS66" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="JT66" t="n">
+      <c r="JT66" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="JU66" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JV66" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -57000,8 +57396,14 @@
       <c r="JS67" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="JT67" t="n">
+      <c r="JT67" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="JU67" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JV67" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -57844,8 +58246,14 @@
       <c r="JS68" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="JT68" t="n">
+      <c r="JT68" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="JU68" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JV68" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -58688,8 +59096,14 @@
       <c r="JS69" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="JT69" t="n">
+      <c r="JT69" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="JU69" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JV69" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -59532,8 +59946,14 @@
       <c r="JS70" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="JT70" t="n">
+      <c r="JT70" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="JU70" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="JV70" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -60376,8 +60796,14 @@
       <c r="JS71" s="1" t="n">
         <v>61.9</v>
       </c>
-      <c r="JT71" t="n">
+      <c r="JT71" s="1" t="n">
         <v>45.5</v>
+      </c>
+      <c r="JU71" s="1" t="n">
+        <v>52.9</v>
+      </c>
+      <c r="JV71" t="n">
+        <v>52.9</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -61220,8 +61646,14 @@
       <c r="JS72" s="1" t="n">
         <v>22.85</v>
       </c>
-      <c r="JT72" t="n">
+      <c r="JT72" s="1" t="n">
         <v>33.4</v>
+      </c>
+      <c r="JU72" s="1" t="n">
+        <v>35.56</v>
+      </c>
+      <c r="JV72" t="n">
+        <v>35.56</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -62064,8 +62496,14 @@
       <c r="JS73" s="1" t="n">
         <v>14.14</v>
       </c>
-      <c r="JT73" t="n">
+      <c r="JT73" s="1" t="n">
         <v>15.18</v>
+      </c>
+      <c r="JU73" s="1" t="n">
+        <v>18.82</v>
+      </c>
+      <c r="JV73" t="n">
+        <v>18.82</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -62908,8 +63346,14 @@
       <c r="JS74" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="JT74" t="n">
+      <c r="JT74" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="JU74" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="JV74" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -63752,7 +64196,13 @@
       <c r="JS75" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="JT75" t="n">
+      <c r="JT75" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="JU75" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="JV75" t="n">
         <v>50</v>
       </c>
     </row>
@@ -64596,8 +65046,14 @@
       <c r="JS76" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="JT76" t="n">
+      <c r="JT76" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="JU76" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="JV76" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -65440,8 +65896,14 @@
       <c r="JS77" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="JT77" t="n">
+      <c r="JT77" s="1" t="n">
         <v>51</v>
+      </c>
+      <c r="JU77" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="JV77" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -66284,8 +66746,14 @@
       <c r="JS78" s="1" t="n">
         <v>2.33</v>
       </c>
-      <c r="JT78" t="n">
+      <c r="JT78" s="1" t="n">
         <v>2.32</v>
+      </c>
+      <c r="JU78" s="1" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="JV78" t="n">
+        <v>3.12</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -67128,8 +67596,14 @@
       <c r="JS79" s="1" t="n">
         <v>3.77</v>
       </c>
-      <c r="JT79" t="n">
+      <c r="JT79" s="1" t="n">
         <v>5.1</v>
+      </c>
+      <c r="JU79" s="1" t="n">
+        <v>5.89</v>
+      </c>
+      <c r="JV79" t="n">
+        <v>5.89</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -67972,8 +68446,14 @@
       <c r="JS80" s="1" t="n">
         <v>38.8</v>
       </c>
-      <c r="JT80" t="n">
+      <c r="JT80" s="1" t="n">
         <v>33.3</v>
+      </c>
+      <c r="JU80" s="1" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="JV80" t="n">
+        <v>24.5</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -68816,8 +69296,14 @@
       <c r="JS81" s="1" t="n">
         <v>26.5</v>
       </c>
-      <c r="JT81" t="n">
+      <c r="JT81" s="1" t="n">
         <v>19.6</v>
+      </c>
+      <c r="JU81" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="JV81" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -69660,8 +70146,14 @@
       <c r="JS82" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="JT82" t="n">
+      <c r="JT82" s="1" t="n">
         <v>188</v>
+      </c>
+      <c r="JU82" s="1" t="n">
+        <v>188.9</v>
+      </c>
+      <c r="JV82" t="n">
+        <v>188.9</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -70504,8 +70996,14 @@
       <c r="JS83" s="1" t="n">
         <v>87.7</v>
       </c>
-      <c r="JT83" t="n">
+      <c r="JT83" s="1" t="n">
         <v>87</v>
+      </c>
+      <c r="JU83" s="1" t="n">
+        <v>87.7</v>
+      </c>
+      <c r="JV83" t="n">
+        <v>87.7</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -71348,8 +71846,14 @@
       <c r="JS84" s="1" t="n">
         <v>26.41</v>
       </c>
-      <c r="JT84" t="n">
+      <c r="JT84" s="1" t="n">
         <v>24.91</v>
+      </c>
+      <c r="JU84" s="1" t="n">
+        <v>25.8</v>
+      </c>
+      <c r="JV84" t="n">
+        <v>25.8</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -72192,8 +72696,14 @@
       <c r="JS85" s="1" t="n">
         <v>108.8</v>
       </c>
-      <c r="JT85" t="n">
+      <c r="JT85" s="1" t="n">
         <v>79.3</v>
+      </c>
+      <c r="JU85" s="1" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="JV85" t="n">
+        <v>87.8</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -73036,8 +73546,14 @@
       <c r="JS86" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JT86" t="n">
+      <c r="JT86" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="JU86" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JV86" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -73880,8 +74396,14 @@
       <c r="JS87" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="JT87" t="n">
+      <c r="JT87" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="JU87" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JV87" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -74724,8 +75246,14 @@
       <c r="JS88" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="JT88" t="n">
+      <c r="JT88" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="JU88" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JV88" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -75568,8 +76096,14 @@
       <c r="JS89" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="JT89" t="n">
+      <c r="JT89" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="JU89" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JV89" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -76412,8 +76946,14 @@
       <c r="JS90" s="1" t="n">
         <v>124</v>
       </c>
-      <c r="JT90" t="n">
+      <c r="JT90" s="1" t="n">
         <v>137</v>
+      </c>
+      <c r="JU90" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="JV90" t="n">
+        <v>130</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -77256,8 +77796,14 @@
       <c r="JS91" s="1" t="n">
         <v>161</v>
       </c>
-      <c r="JT91" t="n">
+      <c r="JT91" s="1" t="n">
         <v>189</v>
+      </c>
+      <c r="JU91" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="JV91" t="n">
+        <v>181</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -78100,8 +78646,14 @@
       <c r="JS92" s="1" t="n">
         <v>215</v>
       </c>
-      <c r="JT92" t="n">
+      <c r="JT92" s="1" t="n">
         <v>239</v>
+      </c>
+      <c r="JU92" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="JV92" t="n">
+        <v>226</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -78944,8 +79496,14 @@
       <c r="JS93" s="1" t="n">
         <v>72.40000000000001</v>
       </c>
-      <c r="JT93" t="n">
+      <c r="JT93" s="1" t="n">
         <v>71.59999999999999</v>
+      </c>
+      <c r="JU93" s="1" t="n">
+        <v>70.59999999999999</v>
+      </c>
+      <c r="JV93" t="n">
+        <v>70.59999999999999</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -79788,7 +80346,13 @@
       <c r="JS94" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="JT94" t="n">
+      <c r="JT94" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="JU94" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="JV94" t="n">
         <v>50</v>
       </c>
     </row>
@@ -80632,8 +81196,14 @@
       <c r="JS95" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JT95" t="n">
+      <c r="JT95" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="JU95" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="JV95" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -81476,8 +82046,14 @@
       <c r="JS96" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JT96" t="n">
+      <c r="JT96" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="JU96" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JV96" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -82320,8 +82896,14 @@
       <c r="JS97" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="JT97" t="n">
+      <c r="JT97" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="JU97" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="JV97" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -83164,8 +83746,14 @@
       <c r="JS98" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="JT98" t="n">
+      <c r="JT98" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="JU98" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="JV98" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -84008,8 +84596,14 @@
       <c r="JS99" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="JT99" t="n">
+      <c r="JT99" s="1" t="n">
         <v>52</v>
+      </c>
+      <c r="JU99" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JV99" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -84852,8 +85446,14 @@
       <c r="JS100" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="JT100" t="n">
+      <c r="JT100" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="JU100" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JV100" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -85696,8 +86296,14 @@
       <c r="JS101" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="JT101" t="n">
+      <c r="JT101" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="JU101" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JV101" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -86540,8 +87146,14 @@
       <c r="JS102" s="1" t="n">
         <v>76.90000000000001</v>
       </c>
-      <c r="JT102" t="n">
+      <c r="JT102" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="JU102" s="1" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="JV102" t="n">
+        <v>66.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
round 6 update and bug fixes.
</commit_message>
<xml_diff>
--- a/AFL_ML/Data/Adelaide_stats.xlsx
+++ b/AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:JV102"/>
+  <dimension ref="A1:JY102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1302,8 +1302,17 @@
       <c r="JU1" s="1" t="n">
         <v>10787</v>
       </c>
-      <c r="JV1" t="n">
+      <c r="JV1" s="1" t="n">
         <v>10787</v>
+      </c>
+      <c r="JW1" s="1" t="n">
+        <v>10800</v>
+      </c>
+      <c r="JX1" s="1" t="n">
+        <v>10800</v>
+      </c>
+      <c r="JY1" t="n">
+        <v>10800</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -2152,7 +2161,16 @@
       <c r="JU2" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="JV2" t="n">
+      <c r="JV2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="JW2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="JX2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="JY2" t="n">
         <v>2023</v>
       </c>
     </row>
@@ -3002,8 +3020,17 @@
       <c r="JU3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="JV3" t="n">
+      <c r="JV3" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="JW3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JX3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JY3" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3852,8 +3879,17 @@
       <c r="JU4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JV4" t="n">
+      <c r="JV4" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="JW4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JX4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JY4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -4702,8 +4738,17 @@
       <c r="JU5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JV5" t="n">
+      <c r="JV5" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="JW5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JX5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JY5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="2">
@@ -5552,8 +5597,17 @@
       <c r="JU6" s="1" t="n">
         <v>118</v>
       </c>
-      <c r="JV6" t="n">
+      <c r="JV6" s="1" t="n">
         <v>118</v>
+      </c>
+      <c r="JW6" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="JX6" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="JY6" t="n">
+        <v>79</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -6402,8 +6456,17 @@
       <c r="JU7" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="JV7" t="n">
+      <c r="JV7" s="1" t="n">
         <v>62</v>
+      </c>
+      <c r="JW7" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="JX7" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="JY7" t="n">
+        <v>76</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -7252,8 +7315,17 @@
       <c r="JU8" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="JV8" t="n">
+      <c r="JV8" s="1" t="n">
         <v>56</v>
+      </c>
+      <c r="JW8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JX8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JY8" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -8102,7 +8174,16 @@
       <c r="JU9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JV9" t="n">
+      <c r="JV9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JW9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JX9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JY9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -8952,8 +9033,17 @@
       <c r="JU10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JV10" t="n">
+      <c r="JV10" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="JW10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JX10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JY10" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -9802,8 +9892,17 @@
       <c r="JU11" s="1" t="n">
         <v>242</v>
       </c>
-      <c r="JV11" t="n">
+      <c r="JV11" s="1" t="n">
         <v>242</v>
+      </c>
+      <c r="JW11" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="JX11" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="JY11" t="n">
+        <v>205</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -10652,8 +10751,17 @@
       <c r="JU12" s="1" t="n">
         <v>156</v>
       </c>
-      <c r="JV12" t="n">
+      <c r="JV12" s="1" t="n">
         <v>156</v>
+      </c>
+      <c r="JW12" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="JX12" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="JY12" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -11502,8 +11610,17 @@
       <c r="JU13" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="JV13" t="n">
+      <c r="JV13" s="1" t="n">
         <v>398</v>
+      </c>
+      <c r="JW13" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="JX13" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="JY13" t="n">
+        <v>355</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -12352,8 +12469,17 @@
       <c r="JU14" s="1" t="n">
         <v>1.55</v>
       </c>
-      <c r="JV14" t="n">
+      <c r="JV14" s="1" t="n">
         <v>1.55</v>
+      </c>
+      <c r="JW14" s="1" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="JX14" s="1" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="JY14" t="n">
+        <v>1.37</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -13202,8 +13328,17 @@
       <c r="JU15" s="1" t="n">
         <v>116</v>
       </c>
-      <c r="JV15" t="n">
+      <c r="JV15" s="1" t="n">
         <v>116</v>
+      </c>
+      <c r="JW15" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="JX15" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="JY15" t="n">
+        <v>79</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -14052,8 +14187,17 @@
       <c r="JU16" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="JV16" t="n">
+      <c r="JV16" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="JW16" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="JX16" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="JY16" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -14902,8 +15046,17 @@
       <c r="JU17" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="JV17" t="n">
+      <c r="JV17" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="JW17" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="JX17" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="JY17" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -15752,8 +15905,17 @@
       <c r="JU18" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="JV18" t="n">
+      <c r="JV18" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="JW18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="JX18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="JY18" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -16602,8 +16764,17 @@
       <c r="JU19" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="JV19" t="n">
+      <c r="JV19" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="JW19" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="JX19" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="JY19" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -17452,8 +17623,17 @@
       <c r="JU20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="JV20" t="n">
+      <c r="JV20" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="JW20" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JX20" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JY20" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -18302,8 +18482,17 @@
       <c r="JU21" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="JV21" t="n">
+      <c r="JV21" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="JW21" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JX21" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JY21" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -19152,8 +19341,17 @@
       <c r="JU22" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="JV22" t="n">
+      <c r="JV22" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="JW22" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JX22" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JY22" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -20002,8 +20200,17 @@
       <c r="JU23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JV23" t="n">
+      <c r="JV23" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="JW23" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JX23" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JY23" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -20852,8 +21059,17 @@
       <c r="JU24" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="JV24" t="n">
+      <c r="JV24" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="JW24" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="JX24" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="JY24" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -21702,8 +21918,17 @@
       <c r="JU25" s="1" t="n">
         <v>64.3</v>
       </c>
-      <c r="JV25" t="n">
+      <c r="JV25" s="1" t="n">
         <v>64.3</v>
+      </c>
+      <c r="JW25" s="1" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="JX25" s="1" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="JY25" t="n">
+        <v>45.8</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -22552,8 +22777,17 @@
       <c r="JU26" s="1" t="n">
         <v>22.11</v>
       </c>
-      <c r="JV26" t="n">
+      <c r="JV26" s="1" t="n">
         <v>22.11</v>
+      </c>
+      <c r="JW26" s="1" t="n">
+        <v>32.27</v>
+      </c>
+      <c r="JX26" s="1" t="n">
+        <v>32.27</v>
+      </c>
+      <c r="JY26" t="n">
+        <v>32.27</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -23402,8 +23636,17 @@
       <c r="JU27" s="1" t="n">
         <v>14.21</v>
       </c>
-      <c r="JV27" t="n">
+      <c r="JV27" s="1" t="n">
         <v>14.21</v>
+      </c>
+      <c r="JW27" s="1" t="n">
+        <v>14.79</v>
+      </c>
+      <c r="JX27" s="1" t="n">
+        <v>14.79</v>
+      </c>
+      <c r="JY27" t="n">
+        <v>14.79</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -24252,8 +24495,17 @@
       <c r="JU28" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="JV28" t="n">
+      <c r="JV28" s="1" t="n">
         <v>37</v>
+      </c>
+      <c r="JW28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JX28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JY28" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -25102,8 +25354,17 @@
       <c r="JU29" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="JV29" t="n">
+      <c r="JV29" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="JW29" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="JX29" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="JY29" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -25952,8 +26213,17 @@
       <c r="JU30" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="JV30" t="n">
+      <c r="JV30" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="JW30" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="JX30" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="JY30" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -26802,8 +27072,17 @@
       <c r="JU31" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="JV31" t="n">
+      <c r="JV31" s="1" t="n">
         <v>51</v>
+      </c>
+      <c r="JW31" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="JX31" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="JY31" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -27652,8 +27931,17 @@
       <c r="JU32" s="1" t="n">
         <v>1.82</v>
       </c>
-      <c r="JV32" t="n">
+      <c r="JV32" s="1" t="n">
         <v>1.82</v>
+      </c>
+      <c r="JW32" s="1" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="JX32" s="1" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="JY32" t="n">
+        <v>2.21</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -28502,8 +28790,17 @@
       <c r="JU33" s="1" t="n">
         <v>2.83</v>
       </c>
-      <c r="JV33" t="n">
+      <c r="JV33" s="1" t="n">
         <v>2.83</v>
+      </c>
+      <c r="JW33" s="1" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="JX33" s="1" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="JY33" t="n">
+        <v>4.82</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -29352,8 +29649,17 @@
       <c r="JU34" s="1" t="n">
         <v>54.9</v>
       </c>
-      <c r="JV34" t="n">
+      <c r="JV34" s="1" t="n">
         <v>54.9</v>
+      </c>
+      <c r="JW34" s="1" t="n">
+        <v>35.8</v>
+      </c>
+      <c r="JX34" s="1" t="n">
+        <v>35.8</v>
+      </c>
+      <c r="JY34" t="n">
+        <v>35.8</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -30202,8 +30508,17 @@
       <c r="JU35" s="1" t="n">
         <v>35.3</v>
       </c>
-      <c r="JV35" t="n">
+      <c r="JV35" s="1" t="n">
         <v>35.3</v>
+      </c>
+      <c r="JW35" s="1" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="JX35" s="1" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="JY35" t="n">
+        <v>20.8</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -31052,7 +31367,16 @@
       <c r="JU36" s="1" t="n">
         <v>187.3</v>
       </c>
-      <c r="JV36" t="n">
+      <c r="JV36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="JW36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="JX36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="JY36" t="n">
         <v>187.3</v>
       </c>
     </row>
@@ -31902,7 +32226,16 @@
       <c r="JU37" s="1" t="n">
         <v>87.59999999999999</v>
       </c>
-      <c r="JV37" t="n">
+      <c r="JV37" s="1" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="JW37" s="1" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="JX37" s="1" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="JY37" t="n">
         <v>87.59999999999999</v>
       </c>
     </row>
@@ -32752,7 +33085,16 @@
       <c r="JU38" s="1" t="n">
         <v>24.74</v>
       </c>
-      <c r="JV38" t="n">
+      <c r="JV38" s="1" t="n">
+        <v>24.74</v>
+      </c>
+      <c r="JW38" s="1" t="n">
+        <v>24.74</v>
+      </c>
+      <c r="JX38" s="1" t="n">
+        <v>24.74</v>
+      </c>
+      <c r="JY38" t="n">
         <v>24.74</v>
       </c>
     </row>
@@ -33602,8 +33944,17 @@
       <c r="JU39" s="1" t="n">
         <v>81.59999999999999</v>
       </c>
-      <c r="JV39" t="n">
+      <c r="JV39" s="1" t="n">
         <v>81.59999999999999</v>
+      </c>
+      <c r="JW39" s="1" t="n">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="JX39" s="1" t="n">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="JY39" t="n">
+        <v>82.59999999999999</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -34452,7 +34803,16 @@
       <c r="JU40" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JV40" t="n">
+      <c r="JV40" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JW40" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JX40" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JY40" t="n">
         <v>9</v>
       </c>
     </row>
@@ -35302,7 +35662,16 @@
       <c r="JU41" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="JV41" t="n">
+      <c r="JV41" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JW41" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JX41" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JY41" t="n">
         <v>10</v>
       </c>
     </row>
@@ -36152,7 +36521,16 @@
       <c r="JU42" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JV42" t="n">
+      <c r="JV42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JW42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JX42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JY42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -37002,7 +37380,16 @@
       <c r="JU43" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JV43" t="n">
+      <c r="JV43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JW43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JX43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JY43" t="n">
         <v>4</v>
       </c>
     </row>
@@ -37852,8 +38239,17 @@
       <c r="JU44" s="1" t="n">
         <v>156</v>
       </c>
-      <c r="JV44" t="n">
+      <c r="JV44" s="1" t="n">
         <v>156</v>
+      </c>
+      <c r="JW44" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="JX44" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="JY44" t="n">
+        <v>145</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -38702,8 +39098,17 @@
       <c r="JU45" s="1" t="n">
         <v>240</v>
       </c>
-      <c r="JV45" t="n">
+      <c r="JV45" s="1" t="n">
         <v>240</v>
+      </c>
+      <c r="JW45" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="JX45" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="JY45" t="n">
+        <v>206</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -39552,8 +39957,17 @@
       <c r="JU46" s="1" t="n">
         <v>302</v>
       </c>
-      <c r="JV46" t="n">
+      <c r="JV46" s="1" t="n">
         <v>302</v>
+      </c>
+      <c r="JW46" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="JX46" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="JY46" t="n">
+        <v>255</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -40402,8 +40816,17 @@
       <c r="JU47" s="1" t="n">
         <v>75.90000000000001</v>
       </c>
-      <c r="JV47" t="n">
+      <c r="JV47" s="1" t="n">
         <v>75.90000000000001</v>
+      </c>
+      <c r="JW47" s="1" t="n">
+        <v>71.8</v>
+      </c>
+      <c r="JX47" s="1" t="n">
+        <v>71.8</v>
+      </c>
+      <c r="JY47" t="n">
+        <v>71.8</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -41252,8 +41675,17 @@
       <c r="JU48" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="JV48" t="n">
+      <c r="JV48" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="JW48" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="JX48" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="JY48" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -42102,8 +42534,17 @@
       <c r="JU49" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="JV49" t="n">
+      <c r="JV49" s="1" t="n">
         <v>19</v>
+      </c>
+      <c r="JW49" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JX49" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JY49" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -42952,8 +43393,17 @@
       <c r="JU50" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="JV50" t="n">
+      <c r="JV50" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="JW50" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="JX50" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="JY50" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -43802,8 +44252,17 @@
       <c r="JU51" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="JV51" t="n">
+      <c r="JV51" s="1" t="n">
         <v>37</v>
+      </c>
+      <c r="JW51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JX51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JY51" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -44652,8 +45111,17 @@
       <c r="JU52" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="JV52" t="n">
+      <c r="JV52" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="JW52" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="JX52" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="JY52" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -45502,8 +45970,17 @@
       <c r="JU53" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="JV53" t="n">
+      <c r="JV53" s="1" t="n">
         <v>52</v>
+      </c>
+      <c r="JW53" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="JX53" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="JY53" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -46352,7 +46829,16 @@
       <c r="JU54" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JV54" t="n">
+      <c r="JV54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JW54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JX54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JY54" t="n">
         <v>3</v>
       </c>
     </row>
@@ -47202,8 +47688,17 @@
       <c r="JU55" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="JV55" t="n">
+      <c r="JV55" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="JW55" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JX55" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JY55" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -48052,8 +48547,17 @@
       <c r="JU56" s="1" t="n">
         <v>83.3</v>
       </c>
-      <c r="JV56" t="n">
+      <c r="JV56" s="1" t="n">
         <v>83.3</v>
+      </c>
+      <c r="JW56" s="1" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="JX56" s="1" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="JY56" t="n">
+        <v>72.7</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -48902,8 +49406,17 @@
       <c r="JU57" s="1" t="n">
         <v>183</v>
       </c>
-      <c r="JV57" t="n">
+      <c r="JV57" s="1" t="n">
         <v>183</v>
+      </c>
+      <c r="JW57" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="JX57" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="JY57" t="n">
+        <v>185</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -49752,8 +50265,17 @@
       <c r="JU58" s="1" t="n">
         <v>137</v>
       </c>
-      <c r="JV58" t="n">
+      <c r="JV58" s="1" t="n">
         <v>137</v>
+      </c>
+      <c r="JW58" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="JX58" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="JY58" t="n">
+        <v>167</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -50602,8 +51124,17 @@
       <c r="JU59" s="1" t="n">
         <v>320</v>
       </c>
-      <c r="JV59" t="n">
+      <c r="JV59" s="1" t="n">
         <v>320</v>
+      </c>
+      <c r="JW59" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="JX59" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="JY59" t="n">
+        <v>352</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -51452,8 +51983,17 @@
       <c r="JU60" s="1" t="n">
         <v>1.34</v>
       </c>
-      <c r="JV60" t="n">
+      <c r="JV60" s="1" t="n">
         <v>1.34</v>
+      </c>
+      <c r="JW60" s="1" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="JX60" s="1" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="JY60" t="n">
+        <v>1.11</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -52302,8 +52842,17 @@
       <c r="JU61" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="JV61" t="n">
+      <c r="JV61" s="1" t="n">
         <v>71</v>
+      </c>
+      <c r="JW61" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="JX61" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="JY61" t="n">
+        <v>78</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -53152,8 +53701,17 @@
       <c r="JU62" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="JV62" t="n">
+      <c r="JV62" s="1" t="n">
         <v>75</v>
+      </c>
+      <c r="JW62" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="JX62" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="JY62" t="n">
+        <v>88</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -54002,8 +54560,17 @@
       <c r="JU63" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="JV63" t="n">
+      <c r="JV63" s="1" t="n">
         <v>29</v>
+      </c>
+      <c r="JW63" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="JX63" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="JY63" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -54852,8 +55419,17 @@
       <c r="JU64" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="JV64" t="n">
+      <c r="JV64" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="JW64" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="JX64" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="JY64" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -55702,8 +56278,17 @@
       <c r="JU65" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="JV65" t="n">
+      <c r="JV65" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="JW65" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="JX65" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="JY65" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -56552,8 +57137,17 @@
       <c r="JU66" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JV66" t="n">
+      <c r="JV66" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="JW66" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JX66" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JY66" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -57402,8 +57996,17 @@
       <c r="JU67" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="JV67" t="n">
+      <c r="JV67" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="JW67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JX67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JY67" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -58252,8 +58855,17 @@
       <c r="JU68" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JV68" t="n">
+      <c r="JV68" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="JW68" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JX68" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JY68" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -59102,8 +59714,17 @@
       <c r="JU69" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JV69" t="n">
+      <c r="JV69" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="JW69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JX69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JY69" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -59952,8 +60573,17 @@
       <c r="JU70" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="JV70" t="n">
+      <c r="JV70" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="JW70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JX70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JY70" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -60802,8 +61432,17 @@
       <c r="JU71" s="1" t="n">
         <v>52.9</v>
       </c>
-      <c r="JV71" t="n">
+      <c r="JV71" s="1" t="n">
         <v>52.9</v>
+      </c>
+      <c r="JW71" s="1" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="JX71" s="1" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="JY71" t="n">
+        <v>52.4</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -61652,8 +62291,17 @@
       <c r="JU72" s="1" t="n">
         <v>35.56</v>
       </c>
-      <c r="JV72" t="n">
+      <c r="JV72" s="1" t="n">
         <v>35.56</v>
+      </c>
+      <c r="JW72" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="JX72" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="JY72" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -62502,8 +63150,17 @@
       <c r="JU73" s="1" t="n">
         <v>18.82</v>
       </c>
-      <c r="JV73" t="n">
+      <c r="JV73" s="1" t="n">
         <v>18.82</v>
+      </c>
+      <c r="JW73" s="1" t="n">
+        <v>16.76</v>
+      </c>
+      <c r="JX73" s="1" t="n">
+        <v>16.76</v>
+      </c>
+      <c r="JY73" t="n">
+        <v>16.76</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -63352,8 +64009,17 @@
       <c r="JU74" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="JV74" t="n">
+      <c r="JV74" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="JW74" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="JX74" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="JY74" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -64202,8 +64868,17 @@
       <c r="JU75" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="JV75" t="n">
+      <c r="JV75" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="JW75" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="JX75" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="JY75" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -65052,8 +65727,17 @@
       <c r="JU76" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="JV76" t="n">
+      <c r="JV76" s="1" t="n">
         <v>32</v>
+      </c>
+      <c r="JW76" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="JX76" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="JY76" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -65902,8 +66586,17 @@
       <c r="JU77" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="JV77" t="n">
+      <c r="JV77" s="1" t="n">
         <v>53</v>
+      </c>
+      <c r="JW77" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JX77" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JY77" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -66752,8 +67445,17 @@
       <c r="JU78" s="1" t="n">
         <v>3.12</v>
       </c>
-      <c r="JV78" t="n">
+      <c r="JV78" s="1" t="n">
         <v>3.12</v>
+      </c>
+      <c r="JW78" s="1" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="JX78" s="1" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="JY78" t="n">
+        <v>2.24</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -67602,8 +68304,17 @@
       <c r="JU79" s="1" t="n">
         <v>5.89</v>
       </c>
-      <c r="JV79" t="n">
+      <c r="JV79" s="1" t="n">
         <v>5.89</v>
+      </c>
+      <c r="JW79" s="1" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="JX79" s="1" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="JY79" t="n">
+        <v>4.27</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -68452,8 +69163,17 @@
       <c r="JU80" s="1" t="n">
         <v>24.5</v>
       </c>
-      <c r="JV80" t="n">
+      <c r="JV80" s="1" t="n">
         <v>24.5</v>
+      </c>
+      <c r="JW80" s="1" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="JX80" s="1" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="JY80" t="n">
+        <v>42.6</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -69302,8 +70022,17 @@
       <c r="JU81" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="JV81" t="n">
+      <c r="JV81" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="JW81" s="1" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="JX81" s="1" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="JY81" t="n">
+        <v>23.4</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -70152,8 +70881,17 @@
       <c r="JU82" s="1" t="n">
         <v>188.9</v>
       </c>
-      <c r="JV82" t="n">
+      <c r="JV82" s="1" t="n">
         <v>188.9</v>
+      </c>
+      <c r="JW82" s="1" t="n">
+        <v>187.7</v>
+      </c>
+      <c r="JX82" s="1" t="n">
+        <v>187.7</v>
+      </c>
+      <c r="JY82" t="n">
+        <v>187.7</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -71002,8 +71740,17 @@
       <c r="JU83" s="1" t="n">
         <v>87.7</v>
       </c>
-      <c r="JV83" t="n">
+      <c r="JV83" s="1" t="n">
         <v>87.7</v>
+      </c>
+      <c r="JW83" s="1" t="n">
+        <v>85.3</v>
+      </c>
+      <c r="JX83" s="1" t="n">
+        <v>85.3</v>
+      </c>
+      <c r="JY83" t="n">
+        <v>85.3</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -71852,8 +72599,17 @@
       <c r="JU84" s="1" t="n">
         <v>25.8</v>
       </c>
-      <c r="JV84" t="n">
+      <c r="JV84" s="1" t="n">
         <v>25.8</v>
+      </c>
+      <c r="JW84" s="1" t="n">
+        <v>24.58</v>
+      </c>
+      <c r="JX84" s="1" t="n">
+        <v>24.58</v>
+      </c>
+      <c r="JY84" t="n">
+        <v>24.58</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -72702,8 +73458,17 @@
       <c r="JU85" s="1" t="n">
         <v>87.8</v>
       </c>
-      <c r="JV85" t="n">
+      <c r="JV85" s="1" t="n">
         <v>87.8</v>
+      </c>
+      <c r="JW85" s="1" t="n">
+        <v>74.2</v>
+      </c>
+      <c r="JX85" s="1" t="n">
+        <v>74.2</v>
+      </c>
+      <c r="JY85" t="n">
+        <v>74.2</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -73552,8 +74317,17 @@
       <c r="JU86" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JV86" t="n">
+      <c r="JV86" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="JW86" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JX86" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JY86" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -74402,8 +75176,17 @@
       <c r="JU87" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="JV87" t="n">
+      <c r="JV87" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="JW87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JX87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JY87" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -75252,8 +76035,17 @@
       <c r="JU88" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="JV88" t="n">
+      <c r="JV88" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="JW88" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JX88" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JY88" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -76102,7 +76894,16 @@
       <c r="JU89" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JV89" t="n">
+      <c r="JV89" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JW89" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JX89" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JY89" t="n">
         <v>3</v>
       </c>
     </row>
@@ -76952,8 +77753,17 @@
       <c r="JU90" s="1" t="n">
         <v>130</v>
       </c>
-      <c r="JV90" t="n">
+      <c r="JV90" s="1" t="n">
         <v>130</v>
+      </c>
+      <c r="JW90" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="JX90" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="JY90" t="n">
+        <v>134</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -77802,8 +78612,17 @@
       <c r="JU91" s="1" t="n">
         <v>181</v>
       </c>
-      <c r="JV91" t="n">
+      <c r="JV91" s="1" t="n">
         <v>181</v>
+      </c>
+      <c r="JW91" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="JX91" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="JY91" t="n">
+        <v>212</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -78652,8 +79471,17 @@
       <c r="JU92" s="1" t="n">
         <v>226</v>
       </c>
-      <c r="JV92" t="n">
+      <c r="JV92" s="1" t="n">
         <v>226</v>
+      </c>
+      <c r="JW92" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="JX92" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="JY92" t="n">
+        <v>265</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -79502,8 +80330,17 @@
       <c r="JU93" s="1" t="n">
         <v>70.59999999999999</v>
       </c>
-      <c r="JV93" t="n">
+      <c r="JV93" s="1" t="n">
         <v>70.59999999999999</v>
+      </c>
+      <c r="JW93" s="1" t="n">
+        <v>75.3</v>
+      </c>
+      <c r="JX93" s="1" t="n">
+        <v>75.3</v>
+      </c>
+      <c r="JY93" t="n">
+        <v>75.3</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -80352,8 +81189,17 @@
       <c r="JU94" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="JV94" t="n">
+      <c r="JV94" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="JW94" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="JX94" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="JY94" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -81202,8 +82048,17 @@
       <c r="JU95" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="JV95" t="n">
+      <c r="JV95" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="JW95" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JX95" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JY95" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -82052,7 +82907,16 @@
       <c r="JU96" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JV96" t="n">
+      <c r="JV96" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JW96" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JX96" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JY96" t="n">
         <v>7</v>
       </c>
     </row>
@@ -82902,8 +83766,17 @@
       <c r="JU97" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="JV97" t="n">
+      <c r="JV97" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="JW97" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="JX97" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="JY97" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -83752,8 +84625,17 @@
       <c r="JU98" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="JV98" t="n">
+      <c r="JV98" s="1" t="n">
         <v>32</v>
+      </c>
+      <c r="JW98" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="JX98" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="JY98" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -84602,8 +85484,17 @@
       <c r="JU99" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="JV99" t="n">
+      <c r="JV99" s="1" t="n">
         <v>47</v>
+      </c>
+      <c r="JW99" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="JX99" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="JY99" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -85452,8 +86343,17 @@
       <c r="JU100" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JV100" t="n">
+      <c r="JV100" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="JW100" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JX100" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JY100" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -86302,8 +87202,17 @@
       <c r="JU101" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="JV101" t="n">
+      <c r="JV101" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="JW101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JX101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JY101" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -87152,8 +88061,17 @@
       <c r="JU102" s="1" t="n">
         <v>66.7</v>
       </c>
-      <c r="JV102" t="n">
+      <c r="JV102" s="1" t="n">
         <v>66.7</v>
+      </c>
+      <c r="JW102" s="1" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="JX102" s="1" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="JY102" t="n">
+        <v>81.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated after round 6 2023. made script to generate pavs per round rather than waiting for HPN to upload pav data.
</commit_message>
<xml_diff>
--- a/AFL_ML/Data/Adelaide_stats.xlsx
+++ b/AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:JY102"/>
+  <dimension ref="A1:KF102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1311,7 +1311,28 @@
       <c r="JX1" s="1" t="n">
         <v>10800</v>
       </c>
-      <c r="JY1" t="n">
+      <c r="JY1" s="1" t="n">
+        <v>10800</v>
+      </c>
+      <c r="JZ1" s="1" t="n">
+        <v>10800</v>
+      </c>
+      <c r="KA1" s="1" t="n">
+        <v>10800</v>
+      </c>
+      <c r="KB1" s="1" t="n">
+        <v>10800</v>
+      </c>
+      <c r="KC1" s="1" t="n">
+        <v>10800</v>
+      </c>
+      <c r="KD1" s="1" t="n">
+        <v>10800</v>
+      </c>
+      <c r="KE1" s="1" t="n">
+        <v>10800</v>
+      </c>
+      <c r="KF1" t="n">
         <v>10800</v>
       </c>
     </row>
@@ -2170,7 +2191,28 @@
       <c r="JX2" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="JY2" t="n">
+      <c r="JY2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="JZ2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="KA2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="KB2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="KC2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="KD2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="KE2" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="KF2" t="n">
         <v>2023</v>
       </c>
     </row>
@@ -3029,7 +3071,28 @@
       <c r="JX3" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="JY3" t="n">
+      <c r="JY3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JZ3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="KA3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="KB3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="KC3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="KD3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="KE3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="KF3" t="n">
         <v>6</v>
       </c>
     </row>
@@ -3888,7 +3951,28 @@
       <c r="JX4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JY4" t="n">
+      <c r="JY4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JZ4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KA4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KB4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KC4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KD4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KE4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KF4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4747,7 +4831,28 @@
       <c r="JX5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JY5" t="n">
+      <c r="JY5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JZ5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KA5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KB5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KC5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KD5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KE5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KF5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5606,7 +5711,28 @@
       <c r="JX6" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="JY6" t="n">
+      <c r="JY6" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="JZ6" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="KA6" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="KB6" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="KC6" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="KD6" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="KE6" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="KF6" t="n">
         <v>79</v>
       </c>
     </row>
@@ -6465,7 +6591,28 @@
       <c r="JX7" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="JY7" t="n">
+      <c r="JY7" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="JZ7" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="KA7" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="KB7" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="KC7" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="KD7" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="KE7" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="KF7" t="n">
         <v>76</v>
       </c>
     </row>
@@ -7324,7 +7471,28 @@
       <c r="JX8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JY8" t="n">
+      <c r="JY8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JZ8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KA8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KB8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KC8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KD8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KE8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KF8" t="n">
         <v>3</v>
       </c>
     </row>
@@ -8183,7 +8351,28 @@
       <c r="JX9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JY9" t="n">
+      <c r="JY9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JZ9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KA9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KB9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KC9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KD9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KE9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KF9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9042,7 +9231,28 @@
       <c r="JX10" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="JY10" t="n">
+      <c r="JY10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JZ10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="KA10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="KB10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="KC10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="KD10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="KE10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="KF10" t="n">
         <v>10</v>
       </c>
     </row>
@@ -9901,7 +10111,28 @@
       <c r="JX11" s="1" t="n">
         <v>205</v>
       </c>
-      <c r="JY11" t="n">
+      <c r="JY11" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="JZ11" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="KA11" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="KB11" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="KC11" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="KD11" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="KE11" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="KF11" t="n">
         <v>205</v>
       </c>
     </row>
@@ -10760,7 +10991,28 @@
       <c r="JX12" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="JY12" t="n">
+      <c r="JY12" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="JZ12" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="KA12" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="KB12" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="KC12" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="KD12" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="KE12" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="KF12" t="n">
         <v>150</v>
       </c>
     </row>
@@ -11619,7 +11871,28 @@
       <c r="JX13" s="1" t="n">
         <v>355</v>
       </c>
-      <c r="JY13" t="n">
+      <c r="JY13" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="JZ13" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="KA13" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="KB13" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="KC13" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="KD13" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="KE13" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="KF13" t="n">
         <v>355</v>
       </c>
     </row>
@@ -12478,7 +12751,28 @@
       <c r="JX14" s="1" t="n">
         <v>1.37</v>
       </c>
-      <c r="JY14" t="n">
+      <c r="JY14" s="1" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="JZ14" s="1" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="KA14" s="1" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="KB14" s="1" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="KC14" s="1" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="KD14" s="1" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="KE14" s="1" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="KF14" t="n">
         <v>1.37</v>
       </c>
     </row>
@@ -13337,7 +13631,28 @@
       <c r="JX15" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="JY15" t="n">
+      <c r="JY15" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="JZ15" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="KA15" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="KB15" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="KC15" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="KD15" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="KE15" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="KF15" t="n">
         <v>79</v>
       </c>
     </row>
@@ -14196,7 +14511,28 @@
       <c r="JX16" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="JY16" t="n">
+      <c r="JY16" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="JZ16" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="KA16" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="KB16" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="KC16" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="KD16" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="KE16" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="KF16" t="n">
         <v>75</v>
       </c>
     </row>
@@ -15055,7 +15391,28 @@
       <c r="JX17" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="JY17" t="n">
+      <c r="JY17" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="JZ17" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="KA17" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="KB17" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="KC17" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="KD17" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="KE17" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="KF17" t="n">
         <v>45</v>
       </c>
     </row>
@@ -15914,7 +16271,28 @@
       <c r="JX18" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="JY18" t="n">
+      <c r="JY18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="JZ18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="KA18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="KB18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="KC18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="KD18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="KE18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="KF18" t="n">
         <v>20</v>
       </c>
     </row>
@@ -16773,7 +17151,28 @@
       <c r="JX19" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="JY19" t="n">
+      <c r="JY19" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="JZ19" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="KA19" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="KB19" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="KC19" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="KD19" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="KE19" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="KF19" t="n">
         <v>19</v>
       </c>
     </row>
@@ -17632,7 +18031,28 @@
       <c r="JX20" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="JY20" t="n">
+      <c r="JY20" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JZ20" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KA20" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KB20" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KC20" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KD20" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KE20" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KF20" t="n">
         <v>11</v>
       </c>
     </row>
@@ -18491,7 +18911,28 @@
       <c r="JX21" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JY21" t="n">
+      <c r="JY21" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JZ21" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KA21" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KB21" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KC21" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KD21" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KE21" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KF21" t="n">
         <v>8</v>
       </c>
     </row>
@@ -19350,7 +19791,28 @@
       <c r="JX22" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JY22" t="n">
+      <c r="JY22" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JZ22" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KA22" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KB22" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KC22" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KD22" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KE22" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KF22" t="n">
         <v>8</v>
       </c>
     </row>
@@ -20209,7 +20671,28 @@
       <c r="JX23" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="JY23" t="n">
+      <c r="JY23" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JZ23" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="KA23" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="KB23" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="KC23" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="KD23" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="KE23" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="KF23" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21068,7 +21551,28 @@
       <c r="JX24" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="JY24" t="n">
+      <c r="JY24" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="JZ24" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="KA24" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="KB24" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="KC24" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="KD24" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="KE24" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="KF24" t="n">
         <v>24</v>
       </c>
     </row>
@@ -21927,7 +22431,28 @@
       <c r="JX25" s="1" t="n">
         <v>45.8</v>
       </c>
-      <c r="JY25" t="n">
+      <c r="JY25" s="1" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="JZ25" s="1" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="KA25" s="1" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="KB25" s="1" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="KC25" s="1" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="KD25" s="1" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="KE25" s="1" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="KF25" t="n">
         <v>45.8</v>
       </c>
     </row>
@@ -22786,7 +23311,28 @@
       <c r="JX26" s="1" t="n">
         <v>32.27</v>
       </c>
-      <c r="JY26" t="n">
+      <c r="JY26" s="1" t="n">
+        <v>32.27</v>
+      </c>
+      <c r="JZ26" s="1" t="n">
+        <v>32.27</v>
+      </c>
+      <c r="KA26" s="1" t="n">
+        <v>32.27</v>
+      </c>
+      <c r="KB26" s="1" t="n">
+        <v>32.27</v>
+      </c>
+      <c r="KC26" s="1" t="n">
+        <v>32.27</v>
+      </c>
+      <c r="KD26" s="1" t="n">
+        <v>32.27</v>
+      </c>
+      <c r="KE26" s="1" t="n">
+        <v>32.27</v>
+      </c>
+      <c r="KF26" t="n">
         <v>32.27</v>
       </c>
     </row>
@@ -23645,7 +24191,28 @@
       <c r="JX27" s="1" t="n">
         <v>14.79</v>
       </c>
-      <c r="JY27" t="n">
+      <c r="JY27" s="1" t="n">
+        <v>14.79</v>
+      </c>
+      <c r="JZ27" s="1" t="n">
+        <v>14.79</v>
+      </c>
+      <c r="KA27" s="1" t="n">
+        <v>14.79</v>
+      </c>
+      <c r="KB27" s="1" t="n">
+        <v>14.79</v>
+      </c>
+      <c r="KC27" s="1" t="n">
+        <v>14.79</v>
+      </c>
+      <c r="KD27" s="1" t="n">
+        <v>14.79</v>
+      </c>
+      <c r="KE27" s="1" t="n">
+        <v>14.79</v>
+      </c>
+      <c r="KF27" t="n">
         <v>14.79</v>
       </c>
     </row>
@@ -24504,7 +25071,28 @@
       <c r="JX28" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="JY28" t="n">
+      <c r="JY28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JZ28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KA28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KB28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KC28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KD28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KE28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KF28" t="n">
         <v>47</v>
       </c>
     </row>
@@ -25363,7 +25951,28 @@
       <c r="JX29" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="JY29" t="n">
+      <c r="JY29" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="JZ29" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="KA29" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="KB29" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="KC29" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="KD29" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="KE29" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="KF29" t="n">
         <v>63</v>
       </c>
     </row>
@@ -26222,7 +26831,28 @@
       <c r="JX30" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="JY30" t="n">
+      <c r="JY30" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="JZ30" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="KA30" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="KB30" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="KC30" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="KD30" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="KE30" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="KF30" t="n">
         <v>34</v>
       </c>
     </row>
@@ -27081,7 +27711,28 @@
       <c r="JX31" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="JY31" t="n">
+      <c r="JY31" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="JZ31" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="KA31" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="KB31" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="KC31" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="KD31" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="KE31" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="KF31" t="n">
         <v>53</v>
       </c>
     </row>
@@ -27940,7 +28591,28 @@
       <c r="JX32" s="1" t="n">
         <v>2.21</v>
       </c>
-      <c r="JY32" t="n">
+      <c r="JY32" s="1" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="JZ32" s="1" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="KA32" s="1" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="KB32" s="1" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="KC32" s="1" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="KD32" s="1" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="KE32" s="1" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="KF32" t="n">
         <v>2.21</v>
       </c>
     </row>
@@ -28799,7 +29471,28 @@
       <c r="JX33" s="1" t="n">
         <v>4.82</v>
       </c>
-      <c r="JY33" t="n">
+      <c r="JY33" s="1" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="JZ33" s="1" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="KA33" s="1" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="KB33" s="1" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="KC33" s="1" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="KD33" s="1" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="KE33" s="1" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="KF33" t="n">
         <v>4.82</v>
       </c>
     </row>
@@ -29658,7 +30351,28 @@
       <c r="JX34" s="1" t="n">
         <v>35.8</v>
       </c>
-      <c r="JY34" t="n">
+      <c r="JY34" s="1" t="n">
+        <v>35.8</v>
+      </c>
+      <c r="JZ34" s="1" t="n">
+        <v>35.8</v>
+      </c>
+      <c r="KA34" s="1" t="n">
+        <v>35.8</v>
+      </c>
+      <c r="KB34" s="1" t="n">
+        <v>35.8</v>
+      </c>
+      <c r="KC34" s="1" t="n">
+        <v>35.8</v>
+      </c>
+      <c r="KD34" s="1" t="n">
+        <v>35.8</v>
+      </c>
+      <c r="KE34" s="1" t="n">
+        <v>35.8</v>
+      </c>
+      <c r="KF34" t="n">
         <v>35.8</v>
       </c>
     </row>
@@ -30517,7 +31231,28 @@
       <c r="JX35" s="1" t="n">
         <v>20.8</v>
       </c>
-      <c r="JY35" t="n">
+      <c r="JY35" s="1" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="JZ35" s="1" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="KA35" s="1" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="KB35" s="1" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="KC35" s="1" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="KD35" s="1" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="KE35" s="1" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="KF35" t="n">
         <v>20.8</v>
       </c>
     </row>
@@ -31376,7 +32111,28 @@
       <c r="JX36" s="1" t="n">
         <v>187.3</v>
       </c>
-      <c r="JY36" t="n">
+      <c r="JY36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="JZ36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="KA36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="KB36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="KC36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="KD36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="KE36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="KF36" t="n">
         <v>187.3</v>
       </c>
     </row>
@@ -32235,7 +32991,28 @@
       <c r="JX37" s="1" t="n">
         <v>87.59999999999999</v>
       </c>
-      <c r="JY37" t="n">
+      <c r="JY37" s="1" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="JZ37" s="1" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="KA37" s="1" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="KB37" s="1" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="KC37" s="1" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="KD37" s="1" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="KE37" s="1" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="KF37" t="n">
         <v>87.59999999999999</v>
       </c>
     </row>
@@ -33094,7 +33871,28 @@
       <c r="JX38" s="1" t="n">
         <v>24.74</v>
       </c>
-      <c r="JY38" t="n">
+      <c r="JY38" s="1" t="n">
+        <v>24.74</v>
+      </c>
+      <c r="JZ38" s="1" t="n">
+        <v>24.74</v>
+      </c>
+      <c r="KA38" s="1" t="n">
+        <v>24.74</v>
+      </c>
+      <c r="KB38" s="1" t="n">
+        <v>24.74</v>
+      </c>
+      <c r="KC38" s="1" t="n">
+        <v>24.74</v>
+      </c>
+      <c r="KD38" s="1" t="n">
+        <v>24.74</v>
+      </c>
+      <c r="KE38" s="1" t="n">
+        <v>24.74</v>
+      </c>
+      <c r="KF38" t="n">
         <v>24.74</v>
       </c>
     </row>
@@ -33953,7 +34751,28 @@
       <c r="JX39" s="1" t="n">
         <v>82.59999999999999</v>
       </c>
-      <c r="JY39" t="n">
+      <c r="JY39" s="1" t="n">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="JZ39" s="1" t="n">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="KA39" s="1" t="n">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="KB39" s="1" t="n">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="KC39" s="1" t="n">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="KD39" s="1" t="n">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="KE39" s="1" t="n">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="KF39" t="n">
         <v>82.59999999999999</v>
       </c>
     </row>
@@ -34812,7 +35631,28 @@
       <c r="JX40" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JY40" t="n">
+      <c r="JY40" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JZ40" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KA40" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KB40" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KC40" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KD40" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KE40" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KF40" t="n">
         <v>9</v>
       </c>
     </row>
@@ -35671,7 +36511,28 @@
       <c r="JX41" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="JY41" t="n">
+      <c r="JY41" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JZ41" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="KA41" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="KB41" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="KC41" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="KD41" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="KE41" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="KF41" t="n">
         <v>10</v>
       </c>
     </row>
@@ -36530,7 +37391,28 @@
       <c r="JX42" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JY42" t="n">
+      <c r="JY42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JZ42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="KA42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="KB42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="KC42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="KD42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="KF42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -37389,7 +38271,28 @@
       <c r="JX43" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JY43" t="n">
+      <c r="JY43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JZ43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="KA43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="KB43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="KC43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="KD43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="KE43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="KF43" t="n">
         <v>4</v>
       </c>
     </row>
@@ -38248,7 +39151,28 @@
       <c r="JX44" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="JY44" t="n">
+      <c r="JY44" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="JZ44" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="KA44" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="KB44" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="KC44" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="KD44" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="KE44" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="KF44" t="n">
         <v>145</v>
       </c>
     </row>
@@ -39107,7 +40031,28 @@
       <c r="JX45" s="1" t="n">
         <v>206</v>
       </c>
-      <c r="JY45" t="n">
+      <c r="JY45" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="JZ45" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="KA45" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="KB45" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="KC45" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="KD45" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="KE45" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="KF45" t="n">
         <v>206</v>
       </c>
     </row>
@@ -39966,7 +40911,28 @@
       <c r="JX46" s="1" t="n">
         <v>255</v>
       </c>
-      <c r="JY46" t="n">
+      <c r="JY46" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="JZ46" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="KA46" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="KB46" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="KC46" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="KD46" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="KE46" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="KF46" t="n">
         <v>255</v>
       </c>
     </row>
@@ -40825,7 +41791,28 @@
       <c r="JX47" s="1" t="n">
         <v>71.8</v>
       </c>
-      <c r="JY47" t="n">
+      <c r="JY47" s="1" t="n">
+        <v>71.8</v>
+      </c>
+      <c r="JZ47" s="1" t="n">
+        <v>71.8</v>
+      </c>
+      <c r="KA47" s="1" t="n">
+        <v>71.8</v>
+      </c>
+      <c r="KB47" s="1" t="n">
+        <v>71.8</v>
+      </c>
+      <c r="KC47" s="1" t="n">
+        <v>71.8</v>
+      </c>
+      <c r="KD47" s="1" t="n">
+        <v>71.8</v>
+      </c>
+      <c r="KE47" s="1" t="n">
+        <v>71.8</v>
+      </c>
+      <c r="KF47" t="n">
         <v>71.8</v>
       </c>
     </row>
@@ -41684,7 +42671,28 @@
       <c r="JX48" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="JY48" t="n">
+      <c r="JY48" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="JZ48" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="KA48" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="KB48" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="KC48" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="KD48" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="KE48" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="KF48" t="n">
         <v>63</v>
       </c>
     </row>
@@ -42543,7 +43551,28 @@
       <c r="JX49" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JY49" t="n">
+      <c r="JY49" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JZ49" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="KA49" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="KB49" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="KC49" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="KD49" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="KE49" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="KF49" t="n">
         <v>7</v>
       </c>
     </row>
@@ -43402,7 +44431,28 @@
       <c r="JX50" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="JY50" t="n">
+      <c r="JY50" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="JZ50" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="KA50" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="KB50" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="KC50" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="KD50" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="KE50" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="KF50" t="n">
         <v>14</v>
       </c>
     </row>
@@ -44261,7 +45311,28 @@
       <c r="JX51" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="JY51" t="n">
+      <c r="JY51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JZ51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KA51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KB51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KC51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KD51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KE51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KF51" t="n">
         <v>47</v>
       </c>
     </row>
@@ -45120,7 +46191,28 @@
       <c r="JX52" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="JY52" t="n">
+      <c r="JY52" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="JZ52" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="KA52" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="KB52" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="KC52" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="KD52" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="KE52" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="KF52" t="n">
         <v>34</v>
       </c>
     </row>
@@ -45979,7 +47071,28 @@
       <c r="JX53" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="JY53" t="n">
+      <c r="JY53" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="JZ53" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="KA53" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="KB53" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="KC53" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="KD53" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="KE53" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="KF53" t="n">
         <v>43</v>
       </c>
     </row>
@@ -46838,7 +47951,28 @@
       <c r="JX54" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JY54" t="n">
+      <c r="JY54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JZ54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KA54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KB54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KC54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KD54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KE54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KF54" t="n">
         <v>3</v>
       </c>
     </row>
@@ -47697,7 +48831,28 @@
       <c r="JX55" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JY55" t="n">
+      <c r="JY55" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JZ55" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KA55" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KB55" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KC55" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KD55" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KE55" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KF55" t="n">
         <v>8</v>
       </c>
     </row>
@@ -48556,7 +49711,28 @@
       <c r="JX56" s="1" t="n">
         <v>72.7</v>
       </c>
-      <c r="JY56" t="n">
+      <c r="JY56" s="1" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="JZ56" s="1" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="KA56" s="1" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="KB56" s="1" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="KC56" s="1" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="KD56" s="1" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="KE56" s="1" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="KF56" t="n">
         <v>72.7</v>
       </c>
     </row>
@@ -49415,7 +50591,28 @@
       <c r="JX57" s="1" t="n">
         <v>185</v>
       </c>
-      <c r="JY57" t="n">
+      <c r="JY57" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="JZ57" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="KA57" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="KB57" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="KC57" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="KD57" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="KE57" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="KF57" t="n">
         <v>185</v>
       </c>
     </row>
@@ -50274,7 +51471,28 @@
       <c r="JX58" s="1" t="n">
         <v>167</v>
       </c>
-      <c r="JY58" t="n">
+      <c r="JY58" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="JZ58" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="KA58" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="KB58" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="KC58" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="KD58" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="KE58" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="KF58" t="n">
         <v>167</v>
       </c>
     </row>
@@ -51133,7 +52351,28 @@
       <c r="JX59" s="1" t="n">
         <v>352</v>
       </c>
-      <c r="JY59" t="n">
+      <c r="JY59" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="JZ59" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="KA59" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="KB59" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="KC59" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="KD59" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="KE59" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="KF59" t="n">
         <v>352</v>
       </c>
     </row>
@@ -51992,7 +53231,28 @@
       <c r="JX60" s="1" t="n">
         <v>1.11</v>
       </c>
-      <c r="JY60" t="n">
+      <c r="JY60" s="1" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="JZ60" s="1" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="KA60" s="1" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="KB60" s="1" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="KC60" s="1" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="KD60" s="1" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="KE60" s="1" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="KF60" t="n">
         <v>1.11</v>
       </c>
     </row>
@@ -52851,7 +54111,28 @@
       <c r="JX61" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="JY61" t="n">
+      <c r="JY61" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="JZ61" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="KA61" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="KB61" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="KC61" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="KD61" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="KE61" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="KF61" t="n">
         <v>78</v>
       </c>
     </row>
@@ -53710,7 +54991,28 @@
       <c r="JX62" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="JY62" t="n">
+      <c r="JY62" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="JZ62" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="KA62" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="KB62" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="KC62" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="KD62" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="KE62" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="KF62" t="n">
         <v>88</v>
       </c>
     </row>
@@ -54569,7 +55871,28 @@
       <c r="JX63" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="JY63" t="n">
+      <c r="JY63" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="JZ63" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="KA63" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="KB63" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="KC63" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="KD63" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="KE63" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="KF63" t="n">
         <v>52</v>
       </c>
     </row>
@@ -55428,7 +56751,28 @@
       <c r="JX64" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="JY64" t="n">
+      <c r="JY64" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="JZ64" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="KA64" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="KB64" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="KC64" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="KD64" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="KE64" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="KF64" t="n">
         <v>19</v>
       </c>
     </row>
@@ -56287,7 +57631,28 @@
       <c r="JX65" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="JY65" t="n">
+      <c r="JY65" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="JZ65" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="KA65" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="KB65" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="KC65" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="KD65" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="KE65" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="KF65" t="n">
         <v>20</v>
       </c>
     </row>
@@ -57146,7 +58511,28 @@
       <c r="JX66" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="JY66" t="n">
+      <c r="JY66" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JZ66" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KA66" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KB66" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KC66" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KD66" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KE66" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KF66" t="n">
         <v>11</v>
       </c>
     </row>
@@ -58005,7 +59391,28 @@
       <c r="JX67" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JY67" t="n">
+      <c r="JY67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JZ67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KA67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KB67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KC67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KD67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KE67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KF67" t="n">
         <v>9</v>
       </c>
     </row>
@@ -58864,7 +60271,28 @@
       <c r="JX68" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JY68" t="n">
+      <c r="JY68" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JZ68" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KA68" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KB68" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KC68" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KD68" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KE68" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KF68" t="n">
         <v>9</v>
       </c>
     </row>
@@ -59723,7 +61151,28 @@
       <c r="JX69" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JY69" t="n">
+      <c r="JY69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JZ69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KA69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KB69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KC69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KD69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KE69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="KF69" t="n">
         <v>1</v>
       </c>
     </row>
@@ -60582,7 +62031,28 @@
       <c r="JX70" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="JY70" t="n">
+      <c r="JY70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JZ70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="KA70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="KB70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="KC70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="KD70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="KE70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="KF70" t="n">
         <v>21</v>
       </c>
     </row>
@@ -61441,7 +62911,28 @@
       <c r="JX71" s="1" t="n">
         <v>52.4</v>
       </c>
-      <c r="JY71" t="n">
+      <c r="JY71" s="1" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="JZ71" s="1" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="KA71" s="1" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="KB71" s="1" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="KC71" s="1" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="KD71" s="1" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="KE71" s="1" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="KF71" t="n">
         <v>52.4</v>
       </c>
     </row>
@@ -62300,7 +63791,28 @@
       <c r="JX72" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="JY72" t="n">
+      <c r="JY72" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="JZ72" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="KA72" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="KB72" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="KC72" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="KD72" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="KE72" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="KF72" t="n">
         <v>32</v>
       </c>
     </row>
@@ -63159,7 +64671,28 @@
       <c r="JX73" s="1" t="n">
         <v>16.76</v>
       </c>
-      <c r="JY73" t="n">
+      <c r="JY73" s="1" t="n">
+        <v>16.76</v>
+      </c>
+      <c r="JZ73" s="1" t="n">
+        <v>16.76</v>
+      </c>
+      <c r="KA73" s="1" t="n">
+        <v>16.76</v>
+      </c>
+      <c r="KB73" s="1" t="n">
+        <v>16.76</v>
+      </c>
+      <c r="KC73" s="1" t="n">
+        <v>16.76</v>
+      </c>
+      <c r="KD73" s="1" t="n">
+        <v>16.76</v>
+      </c>
+      <c r="KE73" s="1" t="n">
+        <v>16.76</v>
+      </c>
+      <c r="KF73" t="n">
         <v>16.76</v>
       </c>
     </row>
@@ -64018,7 +65551,28 @@
       <c r="JX74" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="JY74" t="n">
+      <c r="JY74" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="JZ74" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="KA74" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="KB74" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="KC74" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="KD74" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="KE74" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="KF74" t="n">
         <v>38</v>
       </c>
     </row>
@@ -64877,7 +66431,28 @@
       <c r="JX75" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="JY75" t="n">
+      <c r="JY75" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="JZ75" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="KA75" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="KB75" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="KC75" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="KD75" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="KE75" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="KF75" t="n">
         <v>54</v>
       </c>
     </row>
@@ -65736,7 +67311,28 @@
       <c r="JX76" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="JY76" t="n">
+      <c r="JY76" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="JZ76" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KA76" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KB76" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KC76" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KD76" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KE76" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KF76" t="n">
         <v>42</v>
       </c>
     </row>
@@ -66595,7 +68191,28 @@
       <c r="JX77" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="JY77" t="n">
+      <c r="JY77" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JZ77" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KA77" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KB77" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KC77" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KD77" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KE77" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="KF77" t="n">
         <v>47</v>
       </c>
     </row>
@@ -67454,7 +69071,28 @@
       <c r="JX78" s="1" t="n">
         <v>2.24</v>
       </c>
-      <c r="JY78" t="n">
+      <c r="JY78" s="1" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="JZ78" s="1" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="KA78" s="1" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="KB78" s="1" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="KC78" s="1" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="KD78" s="1" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="KE78" s="1" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="KF78" t="n">
         <v>2.24</v>
       </c>
     </row>
@@ -68313,7 +69951,28 @@
       <c r="JX79" s="1" t="n">
         <v>4.27</v>
       </c>
-      <c r="JY79" t="n">
+      <c r="JY79" s="1" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="JZ79" s="1" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="KA79" s="1" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="KB79" s="1" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="KC79" s="1" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="KD79" s="1" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="KE79" s="1" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="KF79" t="n">
         <v>4.27</v>
       </c>
     </row>
@@ -69172,7 +70831,28 @@
       <c r="JX80" s="1" t="n">
         <v>42.6</v>
       </c>
-      <c r="JY80" t="n">
+      <c r="JY80" s="1" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="JZ80" s="1" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="KA80" s="1" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="KB80" s="1" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="KC80" s="1" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="KD80" s="1" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="KE80" s="1" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="KF80" t="n">
         <v>42.6</v>
       </c>
     </row>
@@ -70031,7 +71711,28 @@
       <c r="JX81" s="1" t="n">
         <v>23.4</v>
       </c>
-      <c r="JY81" t="n">
+      <c r="JY81" s="1" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="JZ81" s="1" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="KA81" s="1" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="KB81" s="1" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="KC81" s="1" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="KD81" s="1" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="KE81" s="1" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="KF81" t="n">
         <v>23.4</v>
       </c>
     </row>
@@ -70890,7 +72591,28 @@
       <c r="JX82" s="1" t="n">
         <v>187.7</v>
       </c>
-      <c r="JY82" t="n">
+      <c r="JY82" s="1" t="n">
+        <v>187.7</v>
+      </c>
+      <c r="JZ82" s="1" t="n">
+        <v>187.7</v>
+      </c>
+      <c r="KA82" s="1" t="n">
+        <v>187.7</v>
+      </c>
+      <c r="KB82" s="1" t="n">
+        <v>187.7</v>
+      </c>
+      <c r="KC82" s="1" t="n">
+        <v>187.7</v>
+      </c>
+      <c r="KD82" s="1" t="n">
+        <v>187.7</v>
+      </c>
+      <c r="KE82" s="1" t="n">
+        <v>187.7</v>
+      </c>
+      <c r="KF82" t="n">
         <v>187.7</v>
       </c>
     </row>
@@ -71749,7 +73471,28 @@
       <c r="JX83" s="1" t="n">
         <v>85.3</v>
       </c>
-      <c r="JY83" t="n">
+      <c r="JY83" s="1" t="n">
+        <v>85.3</v>
+      </c>
+      <c r="JZ83" s="1" t="n">
+        <v>85.3</v>
+      </c>
+      <c r="KA83" s="1" t="n">
+        <v>85.3</v>
+      </c>
+      <c r="KB83" s="1" t="n">
+        <v>85.3</v>
+      </c>
+      <c r="KC83" s="1" t="n">
+        <v>85.3</v>
+      </c>
+      <c r="KD83" s="1" t="n">
+        <v>85.3</v>
+      </c>
+      <c r="KE83" s="1" t="n">
+        <v>85.3</v>
+      </c>
+      <c r="KF83" t="n">
         <v>85.3</v>
       </c>
     </row>
@@ -72608,7 +74351,28 @@
       <c r="JX84" s="1" t="n">
         <v>24.58</v>
       </c>
-      <c r="JY84" t="n">
+      <c r="JY84" s="1" t="n">
+        <v>24.58</v>
+      </c>
+      <c r="JZ84" s="1" t="n">
+        <v>24.58</v>
+      </c>
+      <c r="KA84" s="1" t="n">
+        <v>24.58</v>
+      </c>
+      <c r="KB84" s="1" t="n">
+        <v>24.58</v>
+      </c>
+      <c r="KC84" s="1" t="n">
+        <v>24.58</v>
+      </c>
+      <c r="KD84" s="1" t="n">
+        <v>24.58</v>
+      </c>
+      <c r="KE84" s="1" t="n">
+        <v>24.58</v>
+      </c>
+      <c r="KF84" t="n">
         <v>24.58</v>
       </c>
     </row>
@@ -73467,7 +75231,28 @@
       <c r="JX85" s="1" t="n">
         <v>74.2</v>
       </c>
-      <c r="JY85" t="n">
+      <c r="JY85" s="1" t="n">
+        <v>74.2</v>
+      </c>
+      <c r="JZ85" s="1" t="n">
+        <v>74.2</v>
+      </c>
+      <c r="KA85" s="1" t="n">
+        <v>74.2</v>
+      </c>
+      <c r="KB85" s="1" t="n">
+        <v>74.2</v>
+      </c>
+      <c r="KC85" s="1" t="n">
+        <v>74.2</v>
+      </c>
+      <c r="KD85" s="1" t="n">
+        <v>74.2</v>
+      </c>
+      <c r="KE85" s="1" t="n">
+        <v>74.2</v>
+      </c>
+      <c r="KF85" t="n">
         <v>74.2</v>
       </c>
     </row>
@@ -74326,7 +76111,28 @@
       <c r="JX86" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="JY86" t="n">
+      <c r="JY86" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JZ86" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KA86" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KB86" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KC86" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KD86" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KE86" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="KF86" t="n">
         <v>11</v>
       </c>
     </row>
@@ -75185,7 +76991,28 @@
       <c r="JX87" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="JY87" t="n">
+      <c r="JY87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JZ87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="KA87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="KB87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="KC87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="KD87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="KE87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="KF87" t="n">
         <v>5</v>
       </c>
     </row>
@@ -76044,7 +77871,28 @@
       <c r="JX88" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JY88" t="n">
+      <c r="JY88" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JZ88" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="KA88" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="KB88" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="KC88" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="KD88" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="KE88" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="KF88" t="n">
         <v>4</v>
       </c>
     </row>
@@ -76903,7 +78751,28 @@
       <c r="JX89" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JY89" t="n">
+      <c r="JY89" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JZ89" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KA89" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KB89" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KC89" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KD89" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KE89" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="KF89" t="n">
         <v>3</v>
       </c>
     </row>
@@ -77762,7 +79631,28 @@
       <c r="JX90" s="1" t="n">
         <v>134</v>
       </c>
-      <c r="JY90" t="n">
+      <c r="JY90" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="JZ90" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="KA90" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="KB90" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="KC90" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="KD90" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="KE90" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="KF90" t="n">
         <v>134</v>
       </c>
     </row>
@@ -78621,7 +80511,28 @@
       <c r="JX91" s="1" t="n">
         <v>212</v>
       </c>
-      <c r="JY91" t="n">
+      <c r="JY91" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="JZ91" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="KA91" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="KB91" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="KC91" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="KD91" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="KE91" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="KF91" t="n">
         <v>212</v>
       </c>
     </row>
@@ -79480,7 +81391,28 @@
       <c r="JX92" s="1" t="n">
         <v>265</v>
       </c>
-      <c r="JY92" t="n">
+      <c r="JY92" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="JZ92" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="KA92" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="KB92" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="KC92" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="KD92" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="KE92" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="KF92" t="n">
         <v>265</v>
       </c>
     </row>
@@ -80339,7 +82271,28 @@
       <c r="JX93" s="1" t="n">
         <v>75.3</v>
       </c>
-      <c r="JY93" t="n">
+      <c r="JY93" s="1" t="n">
+        <v>75.3</v>
+      </c>
+      <c r="JZ93" s="1" t="n">
+        <v>75.3</v>
+      </c>
+      <c r="KA93" s="1" t="n">
+        <v>75.3</v>
+      </c>
+      <c r="KB93" s="1" t="n">
+        <v>75.3</v>
+      </c>
+      <c r="KC93" s="1" t="n">
+        <v>75.3</v>
+      </c>
+      <c r="KD93" s="1" t="n">
+        <v>75.3</v>
+      </c>
+      <c r="KE93" s="1" t="n">
+        <v>75.3</v>
+      </c>
+      <c r="KF93" t="n">
         <v>75.3</v>
       </c>
     </row>
@@ -81198,7 +83151,28 @@
       <c r="JX94" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="JY94" t="n">
+      <c r="JY94" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="JZ94" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="KA94" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="KB94" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="KC94" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="KD94" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="KE94" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="KF94" t="n">
         <v>54</v>
       </c>
     </row>
@@ -82057,7 +84031,28 @@
       <c r="JX95" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JY95" t="n">
+      <c r="JY95" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JZ95" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KA95" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KB95" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KC95" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KD95" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KE95" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="KF95" t="n">
         <v>8</v>
       </c>
     </row>
@@ -82916,7 +84911,28 @@
       <c r="JX96" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JY96" t="n">
+      <c r="JY96" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JZ96" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="KA96" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="KB96" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="KC96" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="KD96" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="KE96" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="KF96" t="n">
         <v>7</v>
       </c>
     </row>
@@ -83775,7 +85791,28 @@
       <c r="JX97" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="JY97" t="n">
+      <c r="JY97" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="JZ97" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="KA97" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="KB97" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="KC97" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="KD97" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="KE97" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="KF97" t="n">
         <v>38</v>
       </c>
     </row>
@@ -84634,7 +86671,28 @@
       <c r="JX98" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="JY98" t="n">
+      <c r="JY98" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="JZ98" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KA98" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KB98" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KC98" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KD98" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KE98" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KF98" t="n">
         <v>42</v>
       </c>
     </row>
@@ -85493,7 +87551,28 @@
       <c r="JX99" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="JY99" t="n">
+      <c r="JY99" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="JZ99" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KA99" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KB99" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KC99" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KD99" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KE99" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="KF99" t="n">
         <v>42</v>
       </c>
     </row>
@@ -86352,7 +88431,28 @@
       <c r="JX100" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="JY100" t="n">
+      <c r="JY100" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JZ100" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="KA100" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="KB100" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="KC100" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="KD100" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="KE100" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="KF100" t="n">
         <v>6</v>
       </c>
     </row>
@@ -87211,7 +89311,28 @@
       <c r="JX101" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JY101" t="n">
+      <c r="JY101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JZ101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KA101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KB101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KC101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KD101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KE101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="KF101" t="n">
         <v>9</v>
       </c>
     </row>
@@ -88070,7 +90191,28 @@
       <c r="JX102" s="1" t="n">
         <v>81.8</v>
       </c>
-      <c r="JY102" t="n">
+      <c r="JY102" s="1" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="JZ102" s="1" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="KA102" s="1" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="KB102" s="1" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="KC102" s="1" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="KD102" s="1" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="KE102" s="1" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="KF102" t="n">
         <v>81.8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
round 1 2024 data update
</commit_message>
<xml_diff>
--- a/AFL_ML/Data/Adelaide_stats.xlsx
+++ b/AFL_ML/Data/Adelaide_stats.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:LD102"/>
+  <dimension ref="A1:LE102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="KG88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="KL88" activeCellId="0" sqref="KL88"/>
@@ -1408,8 +1408,11 @@
       <c r="LC1" s="2" t="n">
         <v>10947</v>
       </c>
-      <c r="LD1" t="n">
+      <c r="LD1" s="2" t="n">
         <v>10957</v>
+      </c>
+      <c r="LE1" t="n">
+        <v>10976</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="3">
@@ -2360,7 +2363,10 @@
       <c r="LC2" s="2" t="n">
         <v>2023</v>
       </c>
-      <c r="LD2" t="n">
+      <c r="LD2" s="2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="LE2" t="n">
         <v>2023</v>
       </c>
     </row>
@@ -3312,8 +3318,11 @@
       <c r="LC3" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="LD3" t="n">
+      <c r="LD3" s="2" t="n">
         <v>24</v>
+      </c>
+      <c r="LE3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="3">
@@ -4264,7 +4273,10 @@
       <c r="LC4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="LD4" t="n">
+      <c r="LD4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LE4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5216,8 +5228,11 @@
       <c r="LC5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="LD5" t="n">
+      <c r="LD5" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="LE5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="3">
@@ -6168,8 +6183,11 @@
       <c r="LC6" s="2" t="n">
         <v>73</v>
       </c>
-      <c r="LD6" t="n">
+      <c r="LD6" s="2" t="n">
         <v>123</v>
+      </c>
+      <c r="LE6" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="3">
@@ -7120,8 +7138,11 @@
       <c r="LC7" s="2" t="n">
         <v>74</v>
       </c>
-      <c r="LD7" t="n">
+      <c r="LD7" s="2" t="n">
         <v>78</v>
+      </c>
+      <c r="LE7" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="3">
@@ -8072,8 +8093,11 @@
       <c r="LC8" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="LD8" t="n">
+      <c r="LD8" s="2" t="n">
         <v>45</v>
+      </c>
+      <c r="LE8" t="n">
+        <v>-6</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="3">
@@ -9024,8 +9048,11 @@
       <c r="LC9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="LD9" t="n">
+      <c r="LD9" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="LE9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="3">
@@ -9976,8 +10003,11 @@
       <c r="LC10" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="LD10" t="n">
+      <c r="LD10" s="2" t="n">
         <v>17</v>
+      </c>
+      <c r="LE10" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="3">
@@ -10928,7 +10958,10 @@
       <c r="LC11" s="2" t="n">
         <v>208</v>
       </c>
-      <c r="LD11" t="n">
+      <c r="LD11" s="2" t="n">
+        <v>220</v>
+      </c>
+      <c r="LE11" t="n">
         <v>220</v>
       </c>
     </row>
@@ -11880,8 +11913,11 @@
       <c r="LC12" s="2" t="n">
         <v>147</v>
       </c>
-      <c r="LD12" t="n">
+      <c r="LD12" s="2" t="n">
         <v>179</v>
+      </c>
+      <c r="LE12" t="n">
+        <v>139</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="3">
@@ -12832,8 +12868,11 @@
       <c r="LC13" s="2" t="n">
         <v>355</v>
       </c>
-      <c r="LD13" t="n">
+      <c r="LD13" s="2" t="n">
         <v>399</v>
+      </c>
+      <c r="LE13" t="n">
+        <v>359</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="3">
@@ -13784,8 +13823,11 @@
       <c r="LC14" s="2" t="n">
         <v>1.41</v>
       </c>
-      <c r="LD14" t="n">
+      <c r="LD14" s="2" t="n">
         <v>1.23</v>
+      </c>
+      <c r="LE14" t="n">
+        <v>1.58</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="3">
@@ -14736,8 +14778,11 @@
       <c r="LC15" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="LD15" t="n">
+      <c r="LD15" s="2" t="n">
         <v>100</v>
+      </c>
+      <c r="LE15" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="3">
@@ -15688,8 +15733,11 @@
       <c r="LC16" s="2" t="n">
         <v>81</v>
       </c>
-      <c r="LD16" t="n">
+      <c r="LD16" s="2" t="n">
         <v>45</v>
+      </c>
+      <c r="LE16" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="3">
@@ -16640,8 +16688,11 @@
       <c r="LC17" s="2" t="n">
         <v>61</v>
       </c>
-      <c r="LD17" t="n">
+      <c r="LD17" s="2" t="n">
         <v>33</v>
+      </c>
+      <c r="LE17" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="3">
@@ -17592,8 +17643,11 @@
       <c r="LC18" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="LD18" t="n">
+      <c r="LD18" s="2" t="n">
         <v>11</v>
+      </c>
+      <c r="LE18" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="3">
@@ -18544,8 +18598,11 @@
       <c r="LC19" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="LD19" t="n">
+      <c r="LD19" s="2" t="n">
         <v>22</v>
+      </c>
+      <c r="LE19" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="3">
@@ -19496,8 +19553,11 @@
       <c r="LC20" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="LD20" t="n">
+      <c r="LD20" s="2" t="n">
         <v>17</v>
+      </c>
+      <c r="LE20" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="3">
@@ -20448,8 +20508,11 @@
       <c r="LC21" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="LD21" t="n">
+      <c r="LD21" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="LE21" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="3">
@@ -21400,8 +21463,11 @@
       <c r="LC22" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="LD22" t="n">
+      <c r="LD22" s="2" t="n">
         <v>18</v>
+      </c>
+      <c r="LE22" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="3">
@@ -22352,7 +22418,10 @@
       <c r="LC23" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="LD23" t="n">
+      <c r="LD23" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="LE23" t="n">
         <v>3</v>
       </c>
     </row>
@@ -23304,8 +23373,11 @@
       <c r="LC24" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="LD24" t="n">
+      <c r="LD24" s="2" t="n">
         <v>38</v>
+      </c>
+      <c r="LE24" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="3">
@@ -24256,8 +24328,11 @@
       <c r="LC25" s="2" t="n">
         <v>43.5</v>
       </c>
-      <c r="LD25" t="n">
+      <c r="LD25" s="2" t="n">
         <v>44.7</v>
+      </c>
+      <c r="LE25" t="n">
+        <v>57.1</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="3">
@@ -25208,8 +25283,11 @@
       <c r="LC26" s="2" t="n">
         <v>35.5</v>
       </c>
-      <c r="LD26" t="n">
+      <c r="LD26" s="2" t="n">
         <v>23.47</v>
+      </c>
+      <c r="LE26" t="n">
+        <v>44.88</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="3">
@@ -26160,8 +26238,11 @@
       <c r="LC27" s="2" t="n">
         <v>15.43</v>
       </c>
-      <c r="LD27" t="n">
+      <c r="LD27" s="2" t="n">
         <v>10.5</v>
+      </c>
+      <c r="LE27" t="n">
+        <v>25.64</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="3">
@@ -27112,8 +27193,11 @@
       <c r="LC28" s="2" t="n">
         <v>43</v>
       </c>
-      <c r="LD28" t="n">
+      <c r="LD28" s="2" t="n">
         <v>38</v>
+      </c>
+      <c r="LE28" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="3">
@@ -28064,8 +28148,11 @@
       <c r="LC29" s="2" t="n">
         <v>73</v>
       </c>
-      <c r="LD29" t="n">
+      <c r="LD29" s="2" t="n">
         <v>56</v>
+      </c>
+      <c r="LE29" t="n">
+        <v>66</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="3">
@@ -29016,8 +29103,11 @@
       <c r="LC30" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="LD30" t="n">
+      <c r="LD30" s="2" t="n">
         <v>28</v>
+      </c>
+      <c r="LE30" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="3">
@@ -29968,8 +30058,11 @@
       <c r="LC31" s="2" t="n">
         <v>58</v>
       </c>
-      <c r="LD31" t="n">
+      <c r="LD31" s="2" t="n">
         <v>67</v>
+      </c>
+      <c r="LE31" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="3">
@@ -30920,8 +31013,11 @@
       <c r="LC32" s="2" t="n">
         <v>2.52</v>
       </c>
-      <c r="LD32" t="n">
+      <c r="LD32" s="2" t="n">
         <v>1.76</v>
+      </c>
+      <c r="LE32" t="n">
+        <v>3.86</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="3">
@@ -31872,8 +31968,11 @@
       <c r="LC33" s="2" t="n">
         <v>5.8</v>
       </c>
-      <c r="LD33" t="n">
+      <c r="LD33" s="2" t="n">
         <v>3.94</v>
+      </c>
+      <c r="LE33" t="n">
+        <v>6.75</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="3">
@@ -32824,8 +32923,11 @@
       <c r="LC34" s="2" t="n">
         <v>32.8</v>
       </c>
-      <c r="LD34" t="n">
+      <c r="LD34" s="2" t="n">
         <v>52.2</v>
+      </c>
+      <c r="LE34" t="n">
+        <v>20.4</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="3">
@@ -33776,8 +33878,11 @@
       <c r="LC35" s="2" t="n">
         <v>17.2</v>
       </c>
-      <c r="LD35" t="n">
+      <c r="LD35" s="2" t="n">
         <v>25.4</v>
+      </c>
+      <c r="LE35" t="n">
+        <v>14.8</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="3">
@@ -34728,8 +34833,11 @@
       <c r="LC36" s="2" t="n">
         <v>187.5</v>
       </c>
-      <c r="LD36" t="n">
+      <c r="LD36" s="2" t="n">
         <v>187.6</v>
+      </c>
+      <c r="LE36" t="n">
+        <v>187.2</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="3">
@@ -35680,8 +35788,11 @@
       <c r="LC37" s="2" t="n">
         <v>87.90000000000001</v>
       </c>
-      <c r="LD37" t="n">
+      <c r="LD37" s="2" t="n">
         <v>87.5</v>
+      </c>
+      <c r="LE37" t="n">
+        <v>89</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="3">
@@ -36632,8 +36743,11 @@
       <c r="LC38" s="2" t="n">
         <v>25.24</v>
       </c>
-      <c r="LD38" t="n">
+      <c r="LD38" s="2" t="n">
         <v>24.49</v>
+      </c>
+      <c r="LE38" t="n">
+        <v>24.91</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="3">
@@ -37584,8 +37698,11 @@
       <c r="LC39" s="2" t="n">
         <v>92</v>
       </c>
-      <c r="LD39" t="n">
+      <c r="LD39" s="2" t="n">
         <v>80.90000000000001</v>
+      </c>
+      <c r="LE39" t="n">
+        <v>76.5</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="3">
@@ -38536,8 +38653,11 @@
       <c r="LC40" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="LD40" t="n">
+      <c r="LD40" s="2" t="n">
         <v>11</v>
+      </c>
+      <c r="LE40" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="3">
@@ -39488,8 +39608,11 @@
       <c r="LC41" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LD41" t="n">
+      <c r="LD41" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="LE41" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="3">
@@ -40440,7 +40563,10 @@
       <c r="LC42" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="LD42" t="n">
+      <c r="LD42" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LE42" t="n">
         <v>4</v>
       </c>
     </row>
@@ -41392,8 +41518,11 @@
       <c r="LC43" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="LD43" t="n">
+      <c r="LD43" s="2" t="n">
         <v>3</v>
+      </c>
+      <c r="LE43" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="44" ht="13.8" customHeight="1" s="3">
@@ -42344,8 +42473,11 @@
       <c r="LC44" s="2" t="n">
         <v>165</v>
       </c>
-      <c r="LD44" t="n">
+      <c r="LD44" s="2" t="n">
         <v>136</v>
+      </c>
+      <c r="LE44" t="n">
+        <v>166</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="3">
@@ -43296,8 +43428,11 @@
       <c r="LC45" s="2" t="n">
         <v>187</v>
       </c>
-      <c r="LD45" t="n">
+      <c r="LD45" s="2" t="n">
         <v>260</v>
+      </c>
+      <c r="LE45" t="n">
+        <v>167</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="3">
@@ -44248,8 +44383,11 @@
       <c r="LC46" s="2" t="n">
         <v>242</v>
       </c>
-      <c r="LD46" t="n">
+      <c r="LD46" s="2" t="n">
         <v>295</v>
+      </c>
+      <c r="LE46" t="n">
+        <v>237</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="3">
@@ -45200,8 +45338,11 @@
       <c r="LC47" s="2" t="n">
         <v>68.2</v>
       </c>
-      <c r="LD47" t="n">
+      <c r="LD47" s="2" t="n">
         <v>73.90000000000001</v>
+      </c>
+      <c r="LE47" t="n">
+        <v>66</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="3">
@@ -46152,8 +46293,11 @@
       <c r="LC48" s="2" t="n">
         <v>73</v>
       </c>
-      <c r="LD48" t="n">
+      <c r="LD48" s="2" t="n">
         <v>56</v>
+      </c>
+      <c r="LE48" t="n">
+        <v>66</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="3">
@@ -47104,8 +47248,11 @@
       <c r="LC49" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="LD49" t="n">
+      <c r="LD49" s="2" t="n">
         <v>12</v>
+      </c>
+      <c r="LE49" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="3">
@@ -48056,8 +48203,11 @@
       <c r="LC50" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="LD50" t="n">
+      <c r="LD50" s="2" t="n">
         <v>22</v>
+      </c>
+      <c r="LE50" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="3">
@@ -49008,8 +49158,11 @@
       <c r="LC51" s="2" t="n">
         <v>43</v>
       </c>
-      <c r="LD51" t="n">
+      <c r="LD51" s="2" t="n">
         <v>38</v>
+      </c>
+      <c r="LE51" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="3">
@@ -49960,8 +50113,11 @@
       <c r="LC52" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="LD52" t="n">
+      <c r="LD52" s="2" t="n">
         <v>28</v>
+      </c>
+      <c r="LE52" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="3">
@@ -50912,8 +51068,11 @@
       <c r="LC53" s="2" t="n">
         <v>58</v>
       </c>
-      <c r="LD53" t="n">
+      <c r="LD53" s="2" t="n">
         <v>44</v>
+      </c>
+      <c r="LE53" t="n">
+        <v>62</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="3">
@@ -51864,8 +52023,11 @@
       <c r="LC54" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="LD54" t="n">
+      <c r="LD54" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="LE54" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="3">
@@ -52816,8 +52978,11 @@
       <c r="LC55" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="LD55" t="n">
+      <c r="LD55" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="LE55" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="3">
@@ -53768,8 +53933,11 @@
       <c r="LC56" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="LD56" t="n">
+      <c r="LD56" s="2" t="n">
         <v>58.8</v>
+      </c>
+      <c r="LE56" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="3">
@@ -54720,8 +54888,11 @@
       <c r="LC57" s="2" t="n">
         <v>211</v>
       </c>
-      <c r="LD57" t="n">
+      <c r="LD57" s="2" t="n">
         <v>216</v>
+      </c>
+      <c r="LE57" t="n">
+        <v>227</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="3">
@@ -55672,8 +55843,11 @@
       <c r="LC58" s="2" t="n">
         <v>118</v>
       </c>
-      <c r="LD58" t="n">
+      <c r="LD58" s="2" t="n">
         <v>142</v>
+      </c>
+      <c r="LE58" t="n">
+        <v>139</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="3">
@@ -56624,8 +56798,11 @@
       <c r="LC59" s="2" t="n">
         <v>329</v>
       </c>
-      <c r="LD59" t="n">
+      <c r="LD59" s="2" t="n">
         <v>358</v>
+      </c>
+      <c r="LE59" t="n">
+        <v>366</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="3">
@@ -57576,8 +57753,11 @@
       <c r="LC60" s="2" t="n">
         <v>1.79</v>
       </c>
-      <c r="LD60" t="n">
+      <c r="LD60" s="2" t="n">
         <v>1.52</v>
+      </c>
+      <c r="LE60" t="n">
+        <v>1.63</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="3">
@@ -58528,8 +58708,11 @@
       <c r="LC61" s="2" t="n">
         <v>53</v>
       </c>
-      <c r="LD61" t="n">
+      <c r="LD61" s="2" t="n">
         <v>96</v>
+      </c>
+      <c r="LE61" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="3">
@@ -59480,8 +59663,11 @@
       <c r="LC62" s="2" t="n">
         <v>85</v>
       </c>
-      <c r="LD62" t="n">
+      <c r="LD62" s="2" t="n">
         <v>47</v>
+      </c>
+      <c r="LE62" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="3">
@@ -60432,8 +60618,11 @@
       <c r="LC63" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="LD63" t="n">
+      <c r="LD63" s="2" t="n">
         <v>28</v>
+      </c>
+      <c r="LE63" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="3">
@@ -61384,8 +61573,11 @@
       <c r="LC64" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="LD64" t="n">
+      <c r="LD64" s="2" t="n">
         <v>22</v>
+      </c>
+      <c r="LE64" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="3">
@@ -62336,8 +62528,11 @@
       <c r="LC65" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="LD65" t="n">
+      <c r="LD65" s="2" t="n">
         <v>11</v>
+      </c>
+      <c r="LE65" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="3">
@@ -63288,8 +63483,11 @@
       <c r="LC66" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="LD66" t="n">
+      <c r="LD66" s="2" t="n">
         <v>12</v>
+      </c>
+      <c r="LE66" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="3">
@@ -64240,8 +64438,11 @@
       <c r="LC67" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="LD67" t="n">
+      <c r="LD67" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="LE67" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="3">
@@ -65192,8 +65393,11 @@
       <c r="LC68" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LD68" t="n">
+      <c r="LD68" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="LE68" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="3">
@@ -66144,8 +66348,11 @@
       <c r="LC69" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="LD69" t="n">
+      <c r="LD69" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="LE69" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="3">
@@ -67096,8 +67303,11 @@
       <c r="LC70" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="LD70" t="n">
+      <c r="LD70" s="2" t="n">
         <v>18</v>
+      </c>
+      <c r="LE70" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="3">
@@ -68048,8 +68258,11 @@
       <c r="LC71" s="2" t="n">
         <v>57.9</v>
       </c>
-      <c r="LD71" t="n">
+      <c r="LD71" s="2" t="n">
         <v>66.7</v>
+      </c>
+      <c r="LE71" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="3">
@@ -69000,8 +69213,11 @@
       <c r="LC72" s="2" t="n">
         <v>29.91</v>
       </c>
-      <c r="LD72" t="n">
+      <c r="LD72" s="2" t="n">
         <v>29.83</v>
+      </c>
+      <c r="LE72" t="n">
+        <v>45.75</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="3">
@@ -69952,8 +70168,11 @@
       <c r="LC73" s="2" t="n">
         <v>17.32</v>
       </c>
-      <c r="LD73" t="n">
+      <c r="LD73" s="2" t="n">
         <v>19.89</v>
+      </c>
+      <c r="LE73" t="n">
+        <v>18.3</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="3">
@@ -70904,8 +71123,11 @@
       <c r="LC74" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="LD74" t="n">
+      <c r="LD74" s="2" t="n">
         <v>30</v>
+      </c>
+      <c r="LE74" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="3">
@@ -71856,8 +72078,11 @@
       <c r="LC75" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="LD75" t="n">
+      <c r="LD75" s="2" t="n">
         <v>40</v>
+      </c>
+      <c r="LE75" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="3">
@@ -72808,8 +73033,11 @@
       <c r="LC76" s="2" t="n">
         <v>47</v>
       </c>
-      <c r="LD76" t="n">
+      <c r="LD76" s="2" t="n">
         <v>49</v>
+      </c>
+      <c r="LE76" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="3">
@@ -73760,8 +73988,11 @@
       <c r="LC77" s="2" t="n">
         <v>54</v>
       </c>
-      <c r="LD77" t="n">
+      <c r="LD77" s="2" t="n">
         <v>41</v>
+      </c>
+      <c r="LE77" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="3">
@@ -74712,8 +74943,11 @@
       <c r="LC78" s="2" t="n">
         <v>2.84</v>
       </c>
-      <c r="LD78" t="n">
+      <c r="LD78" s="2" t="n">
         <v>2.28</v>
+      </c>
+      <c r="LE78" t="n">
+        <v>2.55</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="3">
@@ -75664,8 +75898,11 @@
       <c r="LC79" s="2" t="n">
         <v>4.91</v>
       </c>
-      <c r="LD79" t="n">
+      <c r="LD79" s="2" t="n">
         <v>3.42</v>
+      </c>
+      <c r="LE79" t="n">
+        <v>6.38</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="3">
@@ -76616,8 +76853,11 @@
       <c r="LC80" s="2" t="n">
         <v>33.3</v>
       </c>
-      <c r="LD80" t="n">
+      <c r="LD80" s="2" t="n">
         <v>41.5</v>
+      </c>
+      <c r="LE80" t="n">
+        <v>35.3</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="3">
@@ -77568,8 +77808,11 @@
       <c r="LC81" s="2" t="n">
         <v>20.4</v>
       </c>
-      <c r="LD81" t="n">
+      <c r="LD81" s="2" t="n">
         <v>29.3</v>
+      </c>
+      <c r="LE81" t="n">
+        <v>15.7</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="3">
@@ -78520,8 +78763,11 @@
       <c r="LC82" s="2" t="n">
         <v>186.3</v>
       </c>
-      <c r="LD82" t="n">
+      <c r="LD82" s="2" t="n">
         <v>188.2</v>
+      </c>
+      <c r="LE82" t="n">
+        <v>187.4</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="3">
@@ -79472,8 +79718,11 @@
       <c r="LC83" s="2" t="n">
         <v>85.40000000000001</v>
       </c>
-      <c r="LD83" t="n">
+      <c r="LD83" s="2" t="n">
         <v>86.8</v>
+      </c>
+      <c r="LE83" t="n">
+        <v>86.59999999999999</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="3">
@@ -80424,8 +80673,11 @@
       <c r="LC84" s="2" t="n">
         <v>25.91</v>
       </c>
-      <c r="LD84" t="n">
+      <c r="LD84" s="2" t="n">
         <v>25.91</v>
+      </c>
+      <c r="LE84" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="3">
@@ -81376,8 +81628,11 @@
       <c r="LC85" s="2" t="n">
         <v>118.6</v>
       </c>
-      <c r="LD85" t="n">
+      <c r="LD85" s="2" t="n">
         <v>117</v>
+      </c>
+      <c r="LE85" t="n">
+        <v>104.2</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="3">
@@ -82328,8 +82583,11 @@
       <c r="LC86" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="LD86" t="n">
+      <c r="LD86" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="LE86" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="3">
@@ -83280,8 +83538,11 @@
       <c r="LC87" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LD87" t="n">
+      <c r="LD87" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="LE87" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="3">
@@ -84232,7 +84493,10 @@
       <c r="LC88" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="LD88" t="n">
+      <c r="LD88" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LE88" t="n">
         <v>4</v>
       </c>
     </row>
@@ -85184,8 +85448,11 @@
       <c r="LC89" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LD89" t="n">
+      <c r="LD89" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="LE89" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="3">
@@ -86136,8 +86403,11 @@
       <c r="LC90" s="2" t="n">
         <v>165</v>
       </c>
-      <c r="LD90" t="n">
+      <c r="LD90" s="2" t="n">
         <v>121</v>
+      </c>
+      <c r="LE90" t="n">
+        <v>156</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="3">
@@ -87088,8 +87358,11 @@
       <c r="LC91" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="LD91" t="n">
+      <c r="LD91" s="2" t="n">
         <v>220</v>
+      </c>
+      <c r="LE91" t="n">
+        <v>196</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="3">
@@ -88040,8 +88313,11 @@
       <c r="LC92" s="2" t="n">
         <v>198</v>
       </c>
-      <c r="LD92" t="n">
+      <c r="LD92" s="2" t="n">
         <v>266</v>
+      </c>
+      <c r="LE92" t="n">
+        <v>250</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="3">
@@ -88992,8 +89268,11 @@
       <c r="LC93" s="2" t="n">
         <v>60.2</v>
       </c>
-      <c r="LD93" t="n">
+      <c r="LD93" s="2" t="n">
         <v>74.3</v>
+      </c>
+      <c r="LE93" t="n">
+        <v>68.3</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="3">
@@ -89944,8 +90223,11 @@
       <c r="LC94" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="LD94" t="n">
+      <c r="LD94" s="2" t="n">
         <v>40</v>
+      </c>
+      <c r="LE94" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="3">
@@ -90896,8 +91178,11 @@
       <c r="LC95" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="LD95" t="n">
+      <c r="LD95" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="LE95" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="3">
@@ -91848,8 +92133,11 @@
       <c r="LC96" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LD96" t="n">
+      <c r="LD96" s="2" t="n">
         <v>11</v>
+      </c>
+      <c r="LE96" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="3">
@@ -92800,8 +93088,11 @@
       <c r="LC97" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="LD97" t="n">
+      <c r="LD97" s="2" t="n">
         <v>30</v>
+      </c>
+      <c r="LE97" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="3">
@@ -93752,8 +94043,11 @@
       <c r="LC98" s="2" t="n">
         <v>47</v>
       </c>
-      <c r="LD98" t="n">
+      <c r="LD98" s="2" t="n">
         <v>49</v>
+      </c>
+      <c r="LE98" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="3">
@@ -94704,8 +94998,11 @@
       <c r="LC99" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="LD99" t="n">
+      <c r="LD99" s="2" t="n">
         <v>42</v>
+      </c>
+      <c r="LE99" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="3">
@@ -95656,8 +95953,11 @@
       <c r="LC100" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LD100" t="n">
+      <c r="LD100" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="LE100" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="3">
@@ -96608,8 +96908,11 @@
       <c r="LC101" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="LD101" t="n">
+      <c r="LD101" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="LE101" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="3">
@@ -97560,8 +97863,11 @@
       <c r="LC102" s="2" t="n">
         <v>54.5</v>
       </c>
-      <c r="LD102" t="n">
+      <c r="LD102" s="2" t="n">
         <v>58.3</v>
+      </c>
+      <c r="LE102" t="n">
+        <v>62.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>